<commit_message>
modification des conditions de selection de date lors de l'ajotu d'un achat
</commit_message>
<xml_diff>
--- a/public/nom_de_fichier.xlsx
+++ b/public/nom_de_fichier.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
-  <si>
-    <t xml:space="preserve">Activités appro en volume/valeur </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+  <si>
+    <t>COMPTE RENDU ANNUEL</t>
   </si>
   <si>
     <t>Volume</t>
@@ -74,6 +74,9 @@
     <t>Valeur (HT)</t>
   </si>
   <si>
+    <t>Dossiers inférieurs à 2 000,00 € TTC</t>
+  </si>
+  <si>
     <t>MPPA (Année Précédente)</t>
   </si>
   <si>
@@ -107,6 +110,51 @@
     <t>PFAF</t>
   </si>
   <si>
+    <t>Activités appro délais</t>
+  </si>
+  <si>
+    <t>VALEUR</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>MOYENNE</t>
+  </si>
+  <si>
+    <t>MPPA</t>
+  </si>
+  <si>
+    <t>MABC</t>
+  </si>
+  <si>
+    <t>TOTAUX</t>
+  </si>
+  <si>
+    <t>Montant des MPPA</t>
+  </si>
+  <si>
+    <t>Montant des MABC</t>
+  </si>
+  <si>
+    <t>Montant des MABC + MPPA</t>
+  </si>
+  <si>
+    <t>MPPA PME</t>
+  </si>
+  <si>
+    <t>TOP PME VALEUR</t>
+  </si>
+  <si>
+    <t>PME</t>
+  </si>
+  <si>
+    <t>% PME</t>
+  </si>
+  <si>
+    <t>TOP PME VOLUME</t>
+  </si>
+  <si>
     <t>Chorus formul.</t>
   </si>
   <si>
@@ -116,64 +164,58 @@
     <t>Ant. GSBDD</t>
   </si>
   <si>
-    <t>&lt;= 3j / 96.80%</t>
-  </si>
-  <si>
-    <t>&gt; 3j / 3.20%</t>
+    <t>&lt;= 3j / 95.65%</t>
+  </si>
+  <si>
+    <t>&gt; 3j / 4.35%</t>
   </si>
   <si>
     <t>Budget</t>
   </si>
   <si>
-    <t>&lt;= 3j / 96.49%</t>
-  </si>
-  <si>
-    <t>&gt; 3j / 3.51%</t>
-  </si>
-  <si>
-    <t>&lt;= 7j / 89.57%</t>
-  </si>
-  <si>
-    <t>&gt; 7j / 10.43%</t>
+    <t>&lt;= 3j / 91.90%</t>
+  </si>
+  <si>
+    <t>&gt; 3j / 8.10%</t>
+  </si>
+  <si>
+    <t>&lt;= 7j / 64.97%</t>
+  </si>
+  <si>
+    <t>&gt; 7j / 35.03%</t>
   </si>
   <si>
     <t>Fin</t>
   </si>
   <si>
-    <t>&lt; 7j / 97.62%</t>
-  </si>
-  <si>
-    <t>&gt; 7j / 2.38%</t>
-  </si>
-  <si>
-    <t>&lt;= 10j / 91.94%</t>
-  </si>
-  <si>
-    <t>&gt; à 10j / 8.06%</t>
-  </si>
-  <si>
-    <t>&lt;= 14j / 97.42%</t>
-  </si>
-  <si>
-    <t>&gt; à 14j / 2.58%</t>
+    <t>&lt; 7j / 94.51%</t>
+  </si>
+  <si>
+    <t>&gt; 7j / 5.49%</t>
+  </si>
+  <si>
+    <t>&lt;= 10j / 69.20%</t>
+  </si>
+  <si>
+    <t>&gt; à 10j / 30.80%</t>
+  </si>
+  <si>
+    <t>&lt;= 14j / 89.89%</t>
+  </si>
+  <si>
+    <t>&gt; à 14j / 10.11%</t>
   </si>
   <si>
     <t>Délai total</t>
   </si>
   <si>
-    <t>&lt;= 15j / 95.45%</t>
-  </si>
-  <si>
-    <t>&gt; à 15j / 4.55%</t>
-  </si>
-  <si>
-    <t>VALEUR</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>MOYENNE</t>
+    <t>&lt;= 15j / 85.09%</t>
+  </si>
+  <si>
+    <t>&gt; à 15j / 14.91%</t>
+  </si>
+  <si>
+    <t>Activités par type de marché</t>
   </si>
   <si>
     <t>% VALEUR</t>
@@ -182,21 +224,9 @@
     <t>% VOLUME</t>
   </si>
   <si>
-    <t>MPPA</t>
-  </si>
-  <si>
-    <t>MABC</t>
-  </si>
-  <si>
-    <t>TOTAUX</t>
-  </si>
-  <si>
     <t>X &lt;= 1500</t>
   </si>
   <si>
-    <t>Montant des MPPA</t>
-  </si>
-  <si>
     <t>1500 &lt; X &lt;=4000</t>
   </si>
   <si>
@@ -206,30 +236,12 @@
     <t xml:space="preserve">X &gt; </t>
   </si>
   <si>
-    <t>Montant des MABC</t>
-  </si>
-  <si>
-    <t>Montant des MABC + MPPA</t>
-  </si>
-  <si>
-    <t>MPPA PME</t>
-  </si>
-  <si>
-    <t>TOP PME VALEUR</t>
-  </si>
-  <si>
-    <t>PME</t>
+    <t>Activités des PME</t>
   </si>
   <si>
     <t>DEPARTEMENT</t>
   </si>
   <si>
-    <t>% PME</t>
-  </si>
-  <si>
-    <t>TOP PME VOLUME</t>
-  </si>
-  <si>
     <t>VOLUME</t>
   </si>
   <si>
@@ -237,15 +249,6 @@
   </si>
   <si>
     <t>% MPPA</t>
-  </si>
-  <si>
-    <t>Activités appro délais</t>
-  </si>
-  <si>
-    <t>Activités par type de marché</t>
-  </si>
-  <si>
-    <t>Activités des PME</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="18"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -326,27 +329,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -368,17 +356,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="5" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="6" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="7" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="5" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="6" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="7" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -499,40 +490,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>152</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>174</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>183</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -562,40 +553,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>165</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -625,40 +616,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>134</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>231</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>151</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>170</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>93</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>141</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>230</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>206</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>151</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -688,40 +679,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>127</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>146</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -849,17 +840,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Worksheet!$B$131</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -869,10 +849,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 15j / 95.45%</c:v>
+                  <c:v>&lt;= 15j / 85.09%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; à 15j / 4.55%</c:v>
+                  <c:v>&gt; à 15j / 14.91%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -883,10 +863,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>924</c:v>
+                  <c:v>2837</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1014,10 +994,10 @@
               <c:numCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>198</c:v>
+                  <c:v>693</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94</c:v>
+                  <c:v>616</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1151,10 +1131,10 @@
               <c:numCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>182</c:v>
+                  <c:v>644</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>189</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1282,10 +1262,10 @@
               <c:numCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>380</c:v>
+                  <c:v>1337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>283</c:v>
+                  <c:v>881</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1413,7 +1393,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1503443</c:v>
+                  <c:v>7014508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,7 +1408,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1443,7 +1423,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>31561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1643,7 +1623,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>375</c:v>
+                  <c:v>1459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1652,6 +1632,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$L$187</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -1659,6 +1650,12 @@
           <c:val>
             <c:numRef>
               <c:f>Worksheet!$L$186</c:f>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1860,25 +1857,25 @@
                   <c:v>Mai</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>Juin</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>Juillet</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>Août</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>Septembre</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>Octobre</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>Novembre</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>Décembre</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1889,40 +1886,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>143</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>213</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>226</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2050,11 +2047,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Worksheet!$B$16</c:f>
+              <c:f>Worksheet!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TOTAL (Année en cours)</c:v>
+                  <c:v>MPPA (Année en cours)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2108,44 +2105,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Worksheet!$C$16:$N$16</c:f>
+              <c:f>Worksheet!$C$14:$N$14</c:f>
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1202529.02</c:v>
+                  <c:v>3427042.87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6060197.41</c:v>
+                  <c:v>6560707.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11356380.16</c:v>
+                  <c:v>15062208.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12303574.95</c:v>
+                  <c:v>17140160.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12304806.95</c:v>
+                  <c:v>20053863.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12321654.95</c:v>
+                  <c:v>26269693.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12321654.95</c:v>
+                  <c:v>32591922.51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12321654.95</c:v>
+                  <c:v>34953853.13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12321654.95</c:v>
+                  <c:v>41459928.74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12321654.95</c:v>
+                  <c:v>45792861</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12321654.95</c:v>
+                  <c:v>49071173.51</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12321654.95</c:v>
+                  <c:v>61969650.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2156,11 +2153,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Worksheet!$B$19</c:f>
+              <c:f>Worksheet!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TOTAL (Année Précédente)</c:v>
+                  <c:v>MPPA (Année Précédente)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2170,44 +2167,44 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Worksheet!$C$19:$N$19</c:f>
+              <c:f>Worksheet!$C$17:$N$17</c:f>
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3427042.87</c:v>
+                  <c:v>1321328.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6560707.63</c:v>
+                  <c:v>3408628.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15062208.99</c:v>
+                  <c:v>5913110.07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17140160.68</c:v>
+                  <c:v>7607418.46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20053863.04</c:v>
+                  <c:v>10888571.71</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26269693.94</c:v>
+                  <c:v>14512085.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32591922.51</c:v>
+                  <c:v>25615021.51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34953853.13</c:v>
+                  <c:v>28223412.06</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41459928.74</c:v>
+                  <c:v>31072730.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45792861</c:v>
+                  <c:v>34100831.32</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49071173.51</c:v>
+                  <c:v>38781150.42</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61969650.7</c:v>
+                  <c:v>42881828.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2402,40 +2399,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.54</c:v>
+                  <c:v>2.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.31</c:v>
+                  <c:v>1.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56</c:v>
+                  <c:v>1.41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48</c:v>
+                  <c:v>1.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.09</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3.67</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2.98</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.58</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1.38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2465,40 +2462,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>7.05</c:v>
+                  <c:v>9.76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.03</c:v>
+                  <c:v>9.79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.53</c:v>
+                  <c:v>10.29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.08</c:v>
+                  <c:v>8.95</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>13.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9.09</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>8.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7.32</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>7.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>6.66</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>7.43</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>8.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2645,10 +2642,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 3j / 96.80%</c:v>
+                  <c:v>&lt;= 3j / 95.65%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; 3j / 3.20%</c:v>
+                  <c:v>&gt; 3j / 4.35%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2659,10 +2656,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>937</c:v>
+                  <c:v>3189</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2770,10 +2767,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 3j / 96.49%</c:v>
+                  <c:v>&lt;= 3j / 91.90%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; 3j / 3.51%</c:v>
+                  <c:v>&gt; 3j / 8.10%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2784,10 +2781,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>934</c:v>
+                  <c:v>3064</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2895,10 +2892,10 @@
               <c:strCache>
                 <c:ptCount val="376"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 7j / 89.57%</c:v>
+                  <c:v>&lt;= 7j / 64.97%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; 7j / 10.43%</c:v>
+                  <c:v>&gt; 7j / 35.03%</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -4031,10 +4028,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>867</c:v>
+                  <c:v>2166</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101</c:v>
+                  <c:v>1168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4122,17 +4119,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Worksheet!$B$110</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -4142,10 +4128,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt; 7j / 97.62%</c:v>
+                  <c:v>&lt; 7j / 94.51%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; 7j / 2.38%</c:v>
+                  <c:v>&gt; 7j / 5.49%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4156,10 +4142,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>945</c:v>
+                  <c:v>3151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4247,17 +4233,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Worksheet!$G$110</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -4267,10 +4242,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 10j / 91.94%</c:v>
+                  <c:v>&lt;= 10j / 69.20%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; à 10j / 8.06%</c:v>
+                  <c:v>&gt; à 10j / 30.80%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4281,10 +4256,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>890</c:v>
+                  <c:v>2307</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>1027</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4392,10 +4367,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 14j / 97.42%</c:v>
+                  <c:v>&lt;= 14j / 89.89%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; à 14j / 2.58%</c:v>
+                  <c:v>&gt; à 14j / 10.11%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4406,10 +4381,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>943</c:v>
+                  <c:v>2997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4460,13 +4435,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4492,13 +4467,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5340,1498 +5315,2170 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
-        <v>152.0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>174.0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>183.0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>53.0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0.0</v>
+      <c r="C4" s="3">
+        <v>134.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>160.0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>231.0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>125.0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>151.0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>212.0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>170.0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>93.0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>141.0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>230.0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>206.0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>151.0</v>
       </c>
       <c r="O4" s="2">
         <f>SUM(C4:N4)</f>
-        <v>566</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5">
-        <v>104.0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>165.0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>180.0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>42.0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>12.0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0.0</v>
+      <c r="C5" s="4">
+        <v>103.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>116.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>138.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>103.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>131.0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>117.0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>124.0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>99.0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>112.0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>127.0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>146.0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>130.0</v>
       </c>
       <c r="O5" s="2">
         <f>SUM(C5:N5)</f>
-        <v>503</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6">
-        <v>256.0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>339.0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>363.0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>95.0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>15.0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0.0</v>
+      <c r="C6" s="5">
+        <v>237.0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>276.0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>369.0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>228.0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>282.0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>329.0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>294.0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>192.0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>253.0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>357.0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>352.0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>281.0</v>
       </c>
       <c r="O6" s="2">
         <f>SUM(C6:N6)</f>
-        <v>1069</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6">
+        <v>120.0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>138.0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>236.0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>205.0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>227.0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>206.0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>160.0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>99.0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>159.0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>215.0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>208.0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>210.0</v>
+      </c>
+      <c r="O7">
+        <f>SUM(C7:N7)</f>
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7">
+        <v>107.0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>105.0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>152.0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>104.0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>192.0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>148.0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>102.0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>174.0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>139.0</v>
+      </c>
+      <c r="M8" s="7">
         <v>134.0</v>
       </c>
-      <c r="D7" s="7">
-        <v>160.0</v>
-      </c>
-      <c r="E7" s="7">
-        <v>231.0</v>
-      </c>
-      <c r="F7" s="7">
-        <v>125.0</v>
-      </c>
-      <c r="G7" s="7">
-        <v>151.0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>212.0</v>
-      </c>
-      <c r="I7" s="7">
-        <v>170.0</v>
-      </c>
-      <c r="J7" s="7">
-        <v>93.0</v>
-      </c>
-      <c r="K7" s="7">
-        <v>141.0</v>
-      </c>
-      <c r="L7" s="7">
-        <v>230.0</v>
-      </c>
-      <c r="M7" s="7">
-        <v>206.0</v>
-      </c>
-      <c r="N7" s="7">
-        <v>151.0</v>
-      </c>
-      <c r="O7" s="2">
-        <f>SUM(C7:N7)</f>
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="N8" s="7">
         <v>103.0</v>
       </c>
-      <c r="D8" s="8">
-        <v>116.0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>138.0</v>
-      </c>
-      <c r="F8" s="8">
-        <v>103.0</v>
-      </c>
-      <c r="G8" s="8">
-        <v>131.0</v>
-      </c>
-      <c r="H8" s="8">
-        <v>117.0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>124.0</v>
-      </c>
-      <c r="J8" s="8">
-        <v>99.0</v>
-      </c>
-      <c r="K8" s="8">
-        <v>112.0</v>
-      </c>
-      <c r="L8" s="8">
-        <v>127.0</v>
-      </c>
-      <c r="M8" s="8">
-        <v>146.0</v>
-      </c>
-      <c r="N8" s="8">
-        <v>130.0</v>
-      </c>
-      <c r="O8" s="2">
+      <c r="O8">
         <f>SUM(C8:N8)</f>
-        <v>1446</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="9">
-        <v>237.0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>276.0</v>
-      </c>
-      <c r="E9" s="9">
-        <v>369.0</v>
-      </c>
-      <c r="F9" s="9">
-        <v>228.0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>282.0</v>
-      </c>
-      <c r="H9" s="9">
-        <v>329.0</v>
-      </c>
-      <c r="I9" s="9">
-        <v>294.0</v>
-      </c>
-      <c r="J9" s="9">
-        <v>192.0</v>
-      </c>
-      <c r="K9" s="9">
-        <v>253.0</v>
-      </c>
-      <c r="L9" s="9">
-        <v>357.0</v>
-      </c>
-      <c r="M9" s="9">
-        <v>352.0</v>
-      </c>
-      <c r="N9" s="9">
-        <v>281.0</v>
-      </c>
-      <c r="O9" s="2">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="8">
+        <v>227.0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>243.0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>388.0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>309.0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>419.0</v>
+      </c>
+      <c r="H9" s="8">
+        <v>354.0</v>
+      </c>
+      <c r="I9" s="8">
+        <v>262.0</v>
+      </c>
+      <c r="J9" s="8">
+        <v>176.0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>333.0</v>
+      </c>
+      <c r="L9" s="8">
+        <v>354.0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>342.0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>313.0</v>
+      </c>
+      <c r="O9">
         <f>SUM(C9:N9)</f>
-        <v>3450</v>
+        <v>3720</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>573434.82</v>
+      </c>
+      <c r="D12" s="3">
+        <v>745787.03</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1017141.82</v>
+      </c>
+      <c r="F12" s="3">
+        <v>563515.61</v>
+      </c>
+      <c r="G12" s="3">
+        <v>809312.02</v>
+      </c>
+      <c r="H12" s="3">
+        <v>804991.44</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1430406.73</v>
+      </c>
+      <c r="J12" s="3">
+        <v>396459.44</v>
+      </c>
+      <c r="K12" s="3">
+        <v>729066.96</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1531842.53</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1089886.45</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1029487.17</v>
+      </c>
+      <c r="O12" s="2">
+        <f>SUM(C12:N12)</f>
+        <v>10721332.02</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2853608.05</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2387877.73</v>
+      </c>
+      <c r="E13" s="4">
+        <v>7484359.54</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1514436.08</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2104390.34</v>
+      </c>
+      <c r="H13" s="4">
+        <v>5410839.46</v>
+      </c>
+      <c r="I13" s="4">
+        <v>4891821.84</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1965471.18</v>
+      </c>
+      <c r="K13" s="4">
+        <v>5777008.65</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2801089.73</v>
+      </c>
+      <c r="M13" s="4">
+        <v>2188426.06</v>
+      </c>
+      <c r="N13" s="4">
+        <v>11868990.02</v>
+      </c>
+      <c r="O13" s="2">
+        <f>SUM(C13:N13)</f>
+        <v>51248318.68</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4">
-        <v>562465.35</v>
-      </c>
-      <c r="D14" s="4">
-        <v>725052.7</v>
-      </c>
-      <c r="E14" s="4">
-        <v>661291.77</v>
-      </c>
-      <c r="F14" s="4">
-        <v>374227.89</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1232.0</v>
-      </c>
-      <c r="H14" s="4">
-        <v>369.0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="L14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0.0</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>3427042.87</v>
+      </c>
+      <c r="D14" s="5">
+        <v>6560707.63</v>
+      </c>
+      <c r="E14" s="5">
+        <v>15062208.99</v>
+      </c>
+      <c r="F14" s="5">
+        <v>17140160.68</v>
+      </c>
+      <c r="G14" s="5">
+        <v>20053863.04</v>
+      </c>
+      <c r="H14" s="5">
+        <v>26269693.94</v>
+      </c>
+      <c r="I14" s="5">
+        <v>32591922.51</v>
+      </c>
+      <c r="J14" s="5">
+        <v>34953853.13</v>
+      </c>
+      <c r="K14" s="5">
+        <v>41459928.74</v>
+      </c>
+      <c r="L14" s="5">
+        <v>45792861.0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>49071173.51</v>
+      </c>
+      <c r="N14" s="5">
+        <v>61969650.7</v>
       </c>
       <c r="O14" s="2">
         <f>SUM(C14:N14)</f>
-        <v>2324638.71</v>
+        <v>354353066.74</v>
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="5">
-        <v>640063.67</v>
-      </c>
-      <c r="D15" s="5">
-        <v>4132615.69</v>
-      </c>
-      <c r="E15" s="5">
-        <v>4634890.98</v>
-      </c>
-      <c r="F15" s="5">
-        <v>572966.9</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>16479.0</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="L15" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="M15" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="O15" s="2">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="6">
+        <v>312452.75</v>
+      </c>
+      <c r="D15" s="6">
+        <v>557343.77</v>
+      </c>
+      <c r="E15" s="6">
+        <v>982521.22</v>
+      </c>
+      <c r="F15" s="6">
+        <v>842191.86</v>
+      </c>
+      <c r="G15" s="6">
+        <v>729838.13</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1035253.76</v>
+      </c>
+      <c r="I15" s="6">
+        <v>726859.11</v>
+      </c>
+      <c r="J15" s="6">
+        <v>452202.63</v>
+      </c>
+      <c r="K15" s="6">
+        <v>618165.94</v>
+      </c>
+      <c r="L15" s="6">
+        <v>1062671.69</v>
+      </c>
+      <c r="M15" s="6">
+        <v>822340.52</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1187753.03</v>
+      </c>
+      <c r="O15">
         <f>SUM(C15:N15)</f>
-        <v>9997016.24</v>
+        <v>9329594.41</v>
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="B16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1202529.02</v>
-      </c>
-      <c r="D16" s="6">
-        <v>6060197.41</v>
-      </c>
-      <c r="E16" s="6">
-        <v>11356380.16</v>
-      </c>
-      <c r="F16" s="6">
-        <v>12303574.95</v>
-      </c>
-      <c r="G16" s="6">
-        <v>12304806.95</v>
-      </c>
-      <c r="H16" s="6">
-        <v>12321654.95</v>
-      </c>
-      <c r="I16" s="6">
-        <v>12321654.95</v>
-      </c>
-      <c r="J16" s="6">
-        <v>12321654.95</v>
-      </c>
-      <c r="K16" s="6">
-        <v>12321654.95</v>
-      </c>
-      <c r="L16" s="6">
-        <v>12321654.95</v>
-      </c>
-      <c r="M16" s="6">
-        <v>12321654.95</v>
-      </c>
-      <c r="N16" s="6">
-        <v>12321654.95</v>
-      </c>
-      <c r="O16" s="2">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1008875.94</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1529955.59</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1521960.8</v>
+      </c>
+      <c r="F16" s="7">
+        <v>852116.53</v>
+      </c>
+      <c r="G16" s="7">
+        <v>2551315.12</v>
+      </c>
+      <c r="H16" s="7">
+        <v>2588259.65</v>
+      </c>
+      <c r="I16" s="7">
+        <v>10376077.28</v>
+      </c>
+      <c r="J16" s="7">
+        <v>2156187.92</v>
+      </c>
+      <c r="K16" s="7">
+        <v>2231152.02</v>
+      </c>
+      <c r="L16" s="7">
+        <v>1965429.61</v>
+      </c>
+      <c r="M16" s="7">
+        <v>3857978.58</v>
+      </c>
+      <c r="N16" s="7">
+        <v>2912924.86</v>
+      </c>
+      <c r="O16">
         <f>SUM(C16:N16)</f>
-        <v>129479073.14</v>
+        <v>33552233.9</v>
       </c>
     </row>
     <row r="17" spans="1:17">
-      <c r="B17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7">
-        <v>573434.82</v>
-      </c>
-      <c r="D17" s="7">
-        <v>745787.03</v>
-      </c>
-      <c r="E17" s="7">
-        <v>1017141.82</v>
-      </c>
-      <c r="F17" s="7">
-        <v>563515.61</v>
-      </c>
-      <c r="G17" s="7">
-        <v>809312.02</v>
-      </c>
-      <c r="H17" s="7">
-        <v>804991.44</v>
-      </c>
-      <c r="I17" s="7">
-        <v>1430406.73</v>
-      </c>
-      <c r="J17" s="7">
-        <v>396459.44</v>
-      </c>
-      <c r="K17" s="7">
-        <v>729066.96</v>
-      </c>
-      <c r="L17" s="7">
-        <v>1531842.53</v>
-      </c>
-      <c r="M17" s="7">
-        <v>1089886.45</v>
-      </c>
-      <c r="N17" s="7">
-        <v>1029487.17</v>
-      </c>
-      <c r="O17" s="2">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1321328.69</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3408628.05</v>
+      </c>
+      <c r="E17" s="8">
+        <v>5913110.07</v>
+      </c>
+      <c r="F17" s="8">
+        <v>7607418.46</v>
+      </c>
+      <c r="G17" s="8">
+        <v>10888571.71</v>
+      </c>
+      <c r="H17" s="8">
+        <v>14512085.12</v>
+      </c>
+      <c r="I17" s="8">
+        <v>25615021.51</v>
+      </c>
+      <c r="J17" s="8">
+        <v>28223412.06</v>
+      </c>
+      <c r="K17" s="8">
+        <v>31072730.02</v>
+      </c>
+      <c r="L17" s="8">
+        <v>34100831.32</v>
+      </c>
+      <c r="M17" s="8">
+        <v>38781150.42</v>
+      </c>
+      <c r="N17" s="8">
+        <v>42881828.31</v>
+      </c>
+      <c r="O17">
         <f>SUM(C17:N17)</f>
-        <v>10721332.02</v>
+        <v>244326115.74</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="8">
-        <v>2853608.05</v>
-      </c>
-      <c r="D18" s="8">
-        <v>2387877.73</v>
-      </c>
-      <c r="E18" s="8">
-        <v>7484359.54</v>
-      </c>
-      <c r="F18" s="8">
-        <v>1514436.08</v>
-      </c>
-      <c r="G18" s="8">
-        <v>2104390.34</v>
-      </c>
-      <c r="H18" s="8">
-        <v>5410839.46</v>
-      </c>
-      <c r="I18" s="8">
-        <v>4891821.84</v>
-      </c>
-      <c r="J18" s="8">
-        <v>1965471.18</v>
-      </c>
-      <c r="K18" s="8">
-        <v>5777008.65</v>
-      </c>
-      <c r="L18" s="8">
-        <v>2801089.73</v>
-      </c>
-      <c r="M18" s="8">
-        <v>2188426.06</v>
-      </c>
-      <c r="N18" s="8">
-        <v>11868990.02</v>
-      </c>
-      <c r="O18" s="2">
-        <f>SUM(C18:N18)</f>
-        <v>51248318.68</v>
+        <v>19</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="9">
-        <v>3427042.87</v>
-      </c>
-      <c r="D19" s="9">
-        <v>6560707.63</v>
-      </c>
-      <c r="E19" s="9">
-        <v>15062208.99</v>
-      </c>
-      <c r="F19" s="9">
-        <v>17140160.68</v>
-      </c>
-      <c r="G19" s="9">
-        <v>20053863.04</v>
-      </c>
-      <c r="H19" s="9">
-        <v>26269693.94</v>
-      </c>
-      <c r="I19" s="9">
-        <v>32591922.51</v>
-      </c>
-      <c r="J19" s="9">
-        <v>34953853.13</v>
-      </c>
-      <c r="K19" s="9">
-        <v>41459928.74</v>
-      </c>
-      <c r="L19" s="9">
-        <v>45792861.0</v>
-      </c>
-      <c r="M19" s="9">
-        <v>49071173.51</v>
-      </c>
-      <c r="N19" s="9">
-        <v>61969650.7</v>
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3">
+        <v>59</v>
+      </c>
+      <c r="E19" s="3">
+        <v>82</v>
+      </c>
+      <c r="F19" s="3">
+        <v>45</v>
+      </c>
+      <c r="G19" s="3">
+        <v>67</v>
+      </c>
+      <c r="H19" s="3">
+        <v>100</v>
+      </c>
+      <c r="I19" s="3">
+        <v>56</v>
+      </c>
+      <c r="J19" s="3">
+        <v>41</v>
+      </c>
+      <c r="K19" s="3">
+        <v>45</v>
+      </c>
+      <c r="L19" s="3">
+        <v>79</v>
+      </c>
+      <c r="M19" s="3">
+        <v>59</v>
+      </c>
+      <c r="N19" s="3">
+        <v>45</v>
       </c>
       <c r="O19" s="2">
         <f>SUM(C19:N19)</f>
-        <v>354353066.74</v>
-      </c>
+        <v>741</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4">
+        <v>46</v>
+      </c>
+      <c r="D20" s="4">
+        <v>52</v>
+      </c>
+      <c r="E20" s="4">
+        <v>78</v>
+      </c>
+      <c r="F20" s="4">
+        <v>46</v>
+      </c>
+      <c r="G20" s="4">
+        <v>56</v>
+      </c>
+      <c r="H20" s="4">
+        <v>58</v>
+      </c>
+      <c r="I20" s="4">
+        <v>46</v>
+      </c>
+      <c r="J20" s="4">
+        <v>42</v>
+      </c>
+      <c r="K20" s="4">
+        <v>60</v>
+      </c>
+      <c r="L20" s="4">
+        <v>73</v>
+      </c>
+      <c r="M20" s="4">
+        <v>71</v>
+      </c>
+      <c r="N20" s="4">
+        <v>53</v>
+      </c>
+      <c r="O20" s="2">
+        <f>SUM(C20:N20)</f>
+        <v>681</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
+        <v>109</v>
+      </c>
+      <c r="D21" s="5">
+        <v>111</v>
+      </c>
+      <c r="E21" s="5">
+        <v>160</v>
+      </c>
+      <c r="F21" s="5">
+        <v>91</v>
+      </c>
+      <c r="G21" s="5">
+        <v>123</v>
+      </c>
+      <c r="H21" s="5">
+        <v>158</v>
+      </c>
+      <c r="I21" s="5">
+        <v>102</v>
+      </c>
+      <c r="J21" s="5">
+        <v>83</v>
+      </c>
+      <c r="K21" s="5">
+        <v>105</v>
+      </c>
+      <c r="L21" s="5">
+        <v>152</v>
+      </c>
+      <c r="M21" s="5">
+        <v>130</v>
+      </c>
+      <c r="N21" s="5">
+        <v>98</v>
+      </c>
+      <c r="O21" s="2">
+        <f>SUM(C21:N21)</f>
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="9">
+        <v>65</v>
+      </c>
+      <c r="D22" s="9">
+        <v>72</v>
+      </c>
+      <c r="E22" s="9">
+        <v>114</v>
+      </c>
+      <c r="F22" s="9">
+        <v>92</v>
+      </c>
+      <c r="G22" s="9">
+        <v>108</v>
+      </c>
+      <c r="H22" s="9">
+        <v>91</v>
+      </c>
+      <c r="I22" s="9">
+        <v>65</v>
+      </c>
+      <c r="J22" s="9">
+        <v>40</v>
+      </c>
+      <c r="K22" s="9">
+        <v>78</v>
+      </c>
+      <c r="L22" s="9">
+        <v>82</v>
+      </c>
+      <c r="M22" s="9">
+        <v>88</v>
+      </c>
+      <c r="N22" s="9">
+        <v>81</v>
+      </c>
+      <c r="O22" s="2">
+        <f>SUM(C22:N22)</f>
+        <v>976</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="10">
+        <v>54</v>
+      </c>
+      <c r="D23" s="10">
+        <v>50</v>
+      </c>
+      <c r="E23" s="10">
+        <v>55</v>
+      </c>
+      <c r="F23" s="10">
+        <v>60</v>
+      </c>
+      <c r="G23" s="10">
+        <v>100</v>
+      </c>
+      <c r="H23" s="10">
+        <v>86</v>
+      </c>
+      <c r="I23" s="10">
+        <v>52</v>
+      </c>
+      <c r="J23" s="10">
+        <v>37</v>
+      </c>
+      <c r="K23" s="10">
+        <v>107</v>
+      </c>
+      <c r="L23" s="10">
+        <v>75</v>
+      </c>
+      <c r="M23" s="10">
+        <v>58</v>
+      </c>
+      <c r="N23" s="10">
+        <v>43</v>
+      </c>
+      <c r="O23" s="2">
+        <f>SUM(C23:N23)</f>
+        <v>777</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="B24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="11">
+        <v>119</v>
+      </c>
+      <c r="D24" s="11">
+        <v>122</v>
+      </c>
+      <c r="E24" s="11">
+        <v>169</v>
+      </c>
+      <c r="F24" s="11">
+        <v>152</v>
+      </c>
+      <c r="G24" s="11">
+        <v>208</v>
+      </c>
+      <c r="H24" s="11">
+        <v>177</v>
+      </c>
+      <c r="I24" s="11">
+        <v>117</v>
+      </c>
+      <c r="J24" s="11">
+        <v>77</v>
+      </c>
+      <c r="K24" s="11">
+        <v>185</v>
+      </c>
+      <c r="L24" s="11">
+        <v>157</v>
+      </c>
+      <c r="M24" s="11">
+        <v>146</v>
+      </c>
+      <c r="N24" s="11">
+        <v>124</v>
+      </c>
+      <c r="O24" s="2">
+        <f>SUM(C24:N24)</f>
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
     </row>
     <row r="62" spans="1:17">
-      <c r="H62" s="10" t="s">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="B64" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O64" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="B65" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="I65" s="2">
+        <v>1.38</v>
+      </c>
+      <c r="J65" s="2">
+        <v>2.03</v>
+      </c>
+      <c r="K65" s="2">
+        <v>1.69</v>
+      </c>
+      <c r="L65" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="M65" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="N65" s="2">
+        <v>1.48</v>
+      </c>
+      <c r="O65" s="2">
+        <v>0.9825</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="B66" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="2">
+        <v>2.05</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="F66" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="G66" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="H66" s="2">
+        <v>1.58</v>
+      </c>
+      <c r="I66" s="2">
+        <v>2.12</v>
+      </c>
+      <c r="J66" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="K66" s="2">
+        <v>1.29</v>
+      </c>
+      <c r="L66" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="M66" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="N66" s="2">
+        <v>1.07</v>
+      </c>
+      <c r="O66" s="2">
+        <v>1.185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="B67" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="2">
+        <v>2.55</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="E67" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="G67" s="2">
+        <v>1.13</v>
+      </c>
+      <c r="H67" s="2">
+        <v>2.09</v>
+      </c>
+      <c r="I67" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="J67" s="2">
+        <v>3.67</v>
+      </c>
+      <c r="K67" s="2">
+        <v>2.98</v>
+      </c>
+      <c r="L67" s="2">
+        <v>1.58</v>
+      </c>
+      <c r="M67" s="2">
+        <v>1.38</v>
+      </c>
+      <c r="N67" s="2">
+        <v>2.55</v>
+      </c>
+      <c r="O67" s="2">
+        <v>2.1675</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="B68" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="2">
+        <v>7.74</v>
+      </c>
+      <c r="D68" s="2">
+        <v>6.87</v>
+      </c>
+      <c r="E68" s="2">
+        <v>8.16</v>
+      </c>
+      <c r="F68" s="2">
+        <v>7.88</v>
+      </c>
+      <c r="G68" s="2">
+        <v>12.37</v>
+      </c>
+      <c r="H68" s="2">
+        <v>7.21</v>
+      </c>
+      <c r="I68" s="2">
+        <v>6.36</v>
+      </c>
+      <c r="J68" s="2">
+        <v>7.07</v>
+      </c>
+      <c r="K68" s="2">
+        <v>5.38</v>
+      </c>
+      <c r="L68" s="2">
+        <v>5.63</v>
+      </c>
+      <c r="M68" s="2">
+        <v>5.83</v>
+      </c>
+      <c r="N68" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="O68" s="2">
+        <v>7.3083333333333</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="B69" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" s="2">
+        <v>2.02</v>
+      </c>
+      <c r="D69" s="2">
+        <v>2.92</v>
+      </c>
+      <c r="E69" s="2">
+        <v>2.13</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1.07</v>
+      </c>
+      <c r="G69" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="H69" s="2">
+        <v>1.88</v>
+      </c>
+      <c r="I69" s="2">
+        <v>1.66</v>
+      </c>
+      <c r="J69" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="K69" s="2">
+        <v>1.66</v>
+      </c>
+      <c r="L69" s="2">
+        <v>1.03</v>
+      </c>
+      <c r="M69" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="N69" s="2">
+        <v>1.49</v>
+      </c>
+      <c r="O69" s="2">
+        <v>1.545</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="B70" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" s="2">
+        <v>9.76</v>
+      </c>
+      <c r="D70" s="2">
+        <v>9.79</v>
+      </c>
+      <c r="E70" s="2">
+        <v>10.29</v>
+      </c>
+      <c r="F70" s="2">
+        <v>8.95</v>
+      </c>
+      <c r="G70" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H70" s="2">
+        <v>9.09</v>
+      </c>
+      <c r="I70" s="2">
+        <v>8.02</v>
+      </c>
+      <c r="J70" s="2">
+        <v>7.32</v>
+      </c>
+      <c r="K70" s="2">
+        <v>7.04</v>
+      </c>
+      <c r="L70" s="2">
+        <v>6.66</v>
+      </c>
+      <c r="M70" s="2">
+        <v>7.43</v>
+      </c>
+      <c r="N70" s="2">
+        <v>8.69</v>
+      </c>
+      <c r="O70" s="2">
+        <v>8.8533333333333</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="B71" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="2">
+        <v>9.76</v>
+      </c>
+      <c r="D71" s="2">
+        <v>9.79</v>
+      </c>
+      <c r="E71" s="2">
+        <v>10.29</v>
+      </c>
+      <c r="F71" s="2">
+        <v>8.95</v>
+      </c>
+      <c r="G71" s="2">
+        <v>13.21</v>
+      </c>
+      <c r="H71" s="2">
+        <v>9.09</v>
+      </c>
+      <c r="I71" s="2">
+        <v>8.02</v>
+      </c>
+      <c r="J71" s="2">
+        <v>7.32</v>
+      </c>
+      <c r="K71" s="2">
+        <v>7.05</v>
+      </c>
+      <c r="L71" s="2">
+        <v>6.66</v>
+      </c>
+      <c r="M71" s="2">
+        <v>7.43</v>
+      </c>
+      <c r="N71" s="2">
+        <v>8.69</v>
+      </c>
+      <c r="O71" s="2">
+        <v>8.855</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
+      <c r="B72" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72">
+        <v>11.81</v>
+      </c>
+      <c r="D72">
+        <v>10.75</v>
+      </c>
+      <c r="E72">
+        <v>11.05</v>
+      </c>
+      <c r="F72">
+        <v>9.83</v>
+      </c>
+      <c r="G72">
+        <v>13.81</v>
+      </c>
+      <c r="H72">
+        <v>10.67</v>
+      </c>
+      <c r="I72">
+        <v>10.15</v>
+      </c>
+      <c r="J72">
+        <v>8.96</v>
+      </c>
+      <c r="K72">
+        <v>8.34</v>
+      </c>
+      <c r="L72">
+        <v>7.25</v>
+      </c>
+      <c r="M72">
+        <v>8.1</v>
+      </c>
+      <c r="N72">
+        <v>9.76</v>
+      </c>
+      <c r="O72">
+        <v>10.04</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="B73" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73">
+        <v>12.3</v>
+      </c>
+      <c r="D73">
+        <v>11.2</v>
+      </c>
+      <c r="E73">
+        <v>11.7</v>
+      </c>
+      <c r="F73">
+        <v>10.7</v>
+      </c>
+      <c r="G73">
+        <v>14.3</v>
+      </c>
+      <c r="H73">
+        <v>11.2</v>
+      </c>
+      <c r="I73">
+        <v>11.5</v>
+      </c>
+      <c r="J73">
+        <v>11.0</v>
+      </c>
+      <c r="K73">
+        <v>10.0</v>
+      </c>
+      <c r="L73">
+        <v>8.2</v>
+      </c>
+      <c r="M73">
+        <v>8.8</v>
+      </c>
+      <c r="N73">
+        <v>11.2</v>
+      </c>
+      <c r="O73">
+        <v>11.008333333333</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+    </row>
+    <row r="88" spans="1:17">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="L88" s="2"/>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+    </row>
+    <row r="89" spans="1:17">
+      <c r="C89" t="s">
+        <v>49</v>
+      </c>
+      <c r="D89" t="s">
+        <v>50</v>
+      </c>
+      <c r="H89" t="s">
+        <v>52</v>
+      </c>
+      <c r="I89" t="s">
+        <v>53</v>
+      </c>
+      <c r="M89" t="s">
+        <v>54</v>
+      </c>
+      <c r="N89" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17">
+      <c r="B90" t="s">
+        <v>48</v>
+      </c>
+      <c r="C90">
+        <v>3189</v>
+      </c>
+      <c r="D90">
+        <v>145</v>
+      </c>
+      <c r="G90" t="s">
+        <v>51</v>
+      </c>
+      <c r="H90">
+        <v>3064</v>
+      </c>
+      <c r="I90">
+        <v>270</v>
+      </c>
+      <c r="L90" t="s">
+        <v>27</v>
+      </c>
+      <c r="M90">
+        <v>2166</v>
+      </c>
+      <c r="N90">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17">
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="L108" s="2"/>
+      <c r="M108" s="2"/>
+      <c r="N108" s="2"/>
+    </row>
+    <row r="109" spans="1:17">
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="L109" s="2"/>
+      <c r="M109" s="2"/>
+      <c r="N109" s="2"/>
+    </row>
+    <row r="110" spans="1:17">
+      <c r="C110" t="s">
+        <v>57</v>
+      </c>
+      <c r="D110" t="s">
+        <v>58</v>
+      </c>
+      <c r="H110" t="s">
+        <v>59</v>
+      </c>
+      <c r="I110" t="s">
+        <v>60</v>
+      </c>
+      <c r="M110" t="s">
+        <v>61</v>
+      </c>
+      <c r="N110" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17">
+      <c r="B111" t="s">
+        <v>56</v>
+      </c>
+      <c r="C111">
+        <v>3151</v>
+      </c>
+      <c r="D111">
+        <v>183</v>
+      </c>
+      <c r="G111" t="s">
+        <v>46</v>
+      </c>
+      <c r="H111">
+        <v>2307</v>
+      </c>
+      <c r="I111">
+        <v>1027</v>
+      </c>
+      <c r="L111" t="s">
+        <v>30</v>
+      </c>
+      <c r="M111">
+        <v>2997</v>
+      </c>
+      <c r="N111">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17">
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="1:17">
+      <c r="B130" s="2"/>
+      <c r="C130" s="2"/>
+      <c r="D130" s="2"/>
+    </row>
+    <row r="131" spans="1:17">
+      <c r="C131" t="s">
+        <v>64</v>
+      </c>
+      <c r="D131" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17">
+      <c r="B132" t="s">
+        <v>63</v>
+      </c>
+      <c r="C132">
+        <v>2837</v>
+      </c>
+      <c r="D132">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17">
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="2"/>
+      <c r="H151" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17">
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="2"/>
+    </row>
+    <row r="153" spans="1:17">
+      <c r="B153" s="2"/>
+      <c r="C153" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17">
+      <c r="B154" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2">
+        <v>50084826.22</v>
+      </c>
+      <c r="E154" s="2">
+        <v>60316191.86</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17">
+      <c r="B155" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C155" s="2">
+        <v>1929</v>
+      </c>
+      <c r="D155" s="2">
+        <v>1405</v>
+      </c>
+      <c r="E155" s="2">
+        <v>3334</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17">
+      <c r="B156" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C156" s="2">
+        <v>5303.97</v>
+      </c>
+      <c r="D156" s="2">
+        <v>35647.56</v>
+      </c>
+      <c r="E156" s="2">
+        <v>40951.53</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17">
+      <c r="B157" t="s">
+        <v>67</v>
+      </c>
+      <c r="C157">
+        <v>16.96</v>
+      </c>
+      <c r="D157">
+        <v>83.04</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17">
+      <c r="B158" t="s">
+        <v>68</v>
+      </c>
+      <c r="C158">
+        <v>57.86</v>
+      </c>
+      <c r="D158">
+        <v>42.14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17">
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
+      <c r="G159" s="2"/>
+      <c r="H159" s="2"/>
+      <c r="I159" s="2"/>
+      <c r="J159" s="2"/>
+      <c r="L159" s="2"/>
+      <c r="M159" s="2"/>
+      <c r="N159" s="2"/>
+      <c r="O159" s="2"/>
+    </row>
+    <row r="160" spans="1:17">
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2"/>
+      <c r="L160" s="2"/>
+      <c r="M160" s="2"/>
+      <c r="N160" s="2"/>
+      <c r="O160" s="2"/>
+    </row>
+    <row r="161" spans="1:17">
+      <c r="B161" s="2"/>
+      <c r="C161" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="G161" s="2"/>
+      <c r="H161" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I161" s="2"/>
+      <c r="J161" s="2"/>
+      <c r="L161" s="2"/>
+      <c r="M161" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N161" s="2"/>
+      <c r="O161" s="2"/>
+    </row>
+    <row r="162" spans="1:17">
+      <c r="B162" t="s">
+        <v>69</v>
+      </c>
+      <c r="C162" t="s">
+        <v>70</v>
+      </c>
+      <c r="D162" t="s">
+        <v>71</v>
+      </c>
+      <c r="E162" t="s">
+        <v>72</v>
+      </c>
+      <c r="G162" t="s">
+        <v>69</v>
+      </c>
+      <c r="H162" t="s">
+        <v>70</v>
+      </c>
+      <c r="I162" t="s">
+        <v>71</v>
+      </c>
+      <c r="J162" t="s">
+        <v>72</v>
+      </c>
+      <c r="L162" t="s">
+        <v>69</v>
+      </c>
+      <c r="M162" t="s">
+        <v>70</v>
+      </c>
+      <c r="N162" t="s">
+        <v>71</v>
+      </c>
+      <c r="O162" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17">
+      <c r="B163">
+        <v>693</v>
+      </c>
+      <c r="C163">
+        <v>616</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="G163">
+        <v>644</v>
+      </c>
+      <c r="H163">
+        <v>265</v>
+      </c>
+      <c r="I163">
+        <v>0</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+      <c r="L163">
+        <v>1337</v>
+      </c>
+      <c r="M163">
+        <v>881</v>
+      </c>
+      <c r="N163">
+        <v>0</v>
+      </c>
+      <c r="O163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17">
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="2"/>
+    </row>
+    <row r="181" spans="1:17">
+      <c r="B181" s="2"/>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="2"/>
+      <c r="H181" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17">
+      <c r="B182" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17">
+      <c r="B183" s="2"/>
+      <c r="C183" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D183" s="2">
+        <v>7046068.58</v>
+      </c>
+      <c r="E183" s="2">
+        <v>68.87</v>
+      </c>
+      <c r="I183" s="2"/>
+      <c r="J183" s="2"/>
+      <c r="K183" s="2"/>
+    </row>
+    <row r="184" spans="1:17">
+      <c r="B184" s="2"/>
+      <c r="C184" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D184" s="2">
+        <v>1466</v>
+      </c>
+      <c r="E184" s="2">
+        <v>76.0</v>
+      </c>
+      <c r="I184" s="2"/>
+      <c r="J184" s="2"/>
+      <c r="K184" s="2"/>
+    </row>
+    <row r="185" spans="1:17">
+      <c r="B185" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
+      <c r="E185" s="2"/>
+      <c r="I185" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J185" s="2"/>
+      <c r="K185" s="2"/>
+    </row>
+    <row r="186" spans="1:17">
+      <c r="C186" t="s">
+        <v>32</v>
+      </c>
+      <c r="D186">
+        <v>7014508</v>
+      </c>
+      <c r="E186">
+        <v>31561</v>
+      </c>
+      <c r="J186" t="s">
+        <v>75</v>
+      </c>
+      <c r="K186">
+        <v>1459</v>
+      </c>
+      <c r="L186">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17">
+      <c r="C187" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="64" spans="1:17">
-      <c r="B64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="D187"/>
+      <c r="E187">
+        <v>35</v>
+      </c>
+      <c r="J187" t="s">
+        <v>74</v>
+      </c>
+      <c r="K187"/>
+      <c r="L187">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="205" spans="1:17">
+      <c r="B205" s="2"/>
+      <c r="C205" s="2"/>
+      <c r="D205" s="2"/>
+      <c r="E205" s="2"/>
+      <c r="F205" s="2"/>
+      <c r="G205" s="2"/>
+      <c r="H205" s="2"/>
+      <c r="I205" s="2"/>
+      <c r="J205" s="2"/>
+      <c r="K205" s="2"/>
+      <c r="L205" s="2"/>
+      <c r="M205" s="2"/>
+      <c r="N205" s="2"/>
+      <c r="O205" s="2"/>
+    </row>
+    <row r="206" spans="1:17">
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
+      <c r="D206" s="2"/>
+      <c r="E206" s="2"/>
+      <c r="F206" s="2"/>
+      <c r="G206" s="2"/>
+      <c r="H206" s="2"/>
+      <c r="I206" s="2"/>
+      <c r="J206" s="2"/>
+      <c r="K206" s="2"/>
+      <c r="L206" s="2"/>
+      <c r="M206" s="2"/>
+      <c r="N206" s="2"/>
+      <c r="O206" s="2"/>
+    </row>
+    <row r="207" spans="1:17">
+      <c r="B207" s="2"/>
+      <c r="C207" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D207" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E207" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F207" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G207" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H207" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="I207" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J64" s="3" t="s">
+      <c r="J207" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K64" s="3" t="s">
+      <c r="K207" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L64" s="3" t="s">
+      <c r="L207" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M64" s="3" t="s">
+      <c r="M207" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N64" s="3" t="s">
+      <c r="N207" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O64" s="3" t="s">
+      <c r="O207" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
-      <c r="B65" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C65" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="D65" s="3">
-        <v>2.72</v>
-      </c>
-      <c r="E65" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F65" s="3">
-        <v>0.29</v>
-      </c>
-      <c r="G65" s="3">
-        <v>0</v>
-      </c>
-      <c r="H65" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I65" s="3">
-        <v>0</v>
-      </c>
-      <c r="J65" s="3">
-        <v>0</v>
-      </c>
-      <c r="K65" s="3">
-        <v>0</v>
-      </c>
-      <c r="L65" s="3">
-        <v>0</v>
-      </c>
-      <c r="M65" s="3">
-        <v>0</v>
-      </c>
-      <c r="N65" s="3">
-        <v>0</v>
-      </c>
-      <c r="O65" s="3">
-        <v>0.2725</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17">
-      <c r="B66" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C66" s="3">
-        <v>0.38</v>
-      </c>
-      <c r="D66" s="3">
-        <v>0.59</v>
-      </c>
-      <c r="E66" s="3">
-        <v>0.46</v>
-      </c>
-      <c r="F66" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="G66" s="3">
-        <v>0</v>
-      </c>
-      <c r="H66" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I66" s="3">
-        <v>0</v>
-      </c>
-      <c r="J66" s="3">
-        <v>0</v>
-      </c>
-      <c r="K66" s="3">
-        <v>0</v>
-      </c>
-      <c r="L66" s="3">
-        <v>0</v>
-      </c>
-      <c r="M66" s="3">
-        <v>0</v>
-      </c>
-      <c r="N66" s="3">
-        <v>0</v>
-      </c>
-      <c r="O66" s="3">
-        <v>0.135</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17">
-      <c r="B67" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" s="3">
-        <v>0.54</v>
-      </c>
-      <c r="D67" s="3">
-        <v>3.31</v>
-      </c>
-      <c r="E67" s="3">
-        <v>0.56</v>
-      </c>
-      <c r="F67" s="3">
-        <v>0.48</v>
-      </c>
-      <c r="G67" s="3">
-        <v>0</v>
-      </c>
-      <c r="H67" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I67" s="3">
-        <v>0</v>
-      </c>
-      <c r="J67" s="3">
-        <v>0</v>
-      </c>
-      <c r="K67" s="3">
-        <v>0</v>
-      </c>
-      <c r="L67" s="3">
-        <v>0</v>
-      </c>
-      <c r="M67" s="3">
-        <v>0</v>
-      </c>
-      <c r="N67" s="3">
-        <v>0</v>
-      </c>
-      <c r="O67" s="3">
-        <v>0.4075</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17">
-      <c r="B68" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="3">
-        <v>5.16</v>
-      </c>
-      <c r="D68" s="3">
-        <v>4.11</v>
-      </c>
-      <c r="E68" s="3">
-        <v>3.74</v>
-      </c>
-      <c r="F68" s="3">
-        <v>5.14</v>
-      </c>
-      <c r="G68" s="3">
-        <v>0</v>
-      </c>
-      <c r="H68" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I68" s="3">
-        <v>0</v>
-      </c>
-      <c r="J68" s="3">
-        <v>0</v>
-      </c>
-      <c r="K68" s="3">
-        <v>0</v>
-      </c>
-      <c r="L68" s="3">
-        <v>0</v>
-      </c>
-      <c r="M68" s="3">
-        <v>0</v>
-      </c>
-      <c r="N68" s="3">
-        <v>0</v>
-      </c>
-      <c r="O68" s="3">
-        <v>1.5125</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17">
-      <c r="B69" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C69" s="3">
-        <v>1.89</v>
-      </c>
-      <c r="D69" s="3">
-        <v>0.92</v>
-      </c>
-      <c r="E69" s="3">
-        <v>0.79</v>
-      </c>
-      <c r="F69" s="3">
-        <v>0.94</v>
-      </c>
-      <c r="G69" s="3">
-        <v>0</v>
-      </c>
-      <c r="H69" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I69" s="3">
-        <v>0</v>
-      </c>
-      <c r="J69" s="3">
-        <v>0</v>
-      </c>
-      <c r="K69" s="3">
-        <v>0</v>
-      </c>
-      <c r="L69" s="3">
-        <v>0</v>
-      </c>
-      <c r="M69" s="3">
-        <v>0</v>
-      </c>
-      <c r="N69" s="3">
-        <v>0</v>
-      </c>
-      <c r="O69" s="3">
-        <v>0.37833333333333</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17">
-      <c r="B70" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C70" s="3">
-        <v>7.05</v>
-      </c>
-      <c r="D70" s="3">
-        <v>5.03</v>
-      </c>
-      <c r="E70" s="3">
-        <v>4.53</v>
-      </c>
-      <c r="F70" s="3">
-        <v>6.08</v>
-      </c>
-      <c r="G70" s="3">
-        <v>0</v>
-      </c>
-      <c r="H70" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I70" s="3">
-        <v>0</v>
-      </c>
-      <c r="J70" s="3">
-        <v>0</v>
-      </c>
-      <c r="K70" s="3">
-        <v>0</v>
-      </c>
-      <c r="L70" s="3">
-        <v>0</v>
-      </c>
-      <c r="M70" s="3">
-        <v>0</v>
-      </c>
-      <c r="N70" s="3">
-        <v>0</v>
-      </c>
-      <c r="O70" s="3">
-        <v>1.8908333333333</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17">
-      <c r="B71" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" s="3">
-        <v>7.05</v>
-      </c>
-      <c r="D71" s="3">
-        <v>5.03</v>
-      </c>
-      <c r="E71" s="3">
-        <v>4.54</v>
-      </c>
-      <c r="F71" s="3">
-        <v>6.08</v>
-      </c>
-      <c r="G71" s="3">
-        <v>0</v>
-      </c>
-      <c r="H71" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I71" s="3">
-        <v>0</v>
-      </c>
-      <c r="J71" s="3">
-        <v>0</v>
-      </c>
-      <c r="K71" s="3">
-        <v>0</v>
-      </c>
-      <c r="L71" s="3">
-        <v>0</v>
-      </c>
-      <c r="M71" s="3">
-        <v>0</v>
-      </c>
-      <c r="N71" s="3">
-        <v>0</v>
-      </c>
-      <c r="O71" s="3">
-        <v>1.8916666666667</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17">
-      <c r="B72" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72" s="3">
-        <v>7.43</v>
-      </c>
-      <c r="D72" s="3">
-        <v>5.62</v>
-      </c>
-      <c r="E72" s="3">
-        <v>4.99</v>
-      </c>
-      <c r="F72" s="3">
-        <v>6.27</v>
-      </c>
-      <c r="G72" s="3">
-        <v>0</v>
-      </c>
-      <c r="H72" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I72" s="3">
-        <v>0</v>
-      </c>
-      <c r="J72" s="3">
-        <v>0</v>
-      </c>
-      <c r="K72" s="3">
-        <v>0</v>
-      </c>
-      <c r="L72" s="3">
-        <v>0</v>
-      </c>
-      <c r="M72" s="3">
-        <v>0</v>
-      </c>
-      <c r="N72" s="3">
-        <v>0</v>
-      </c>
-      <c r="O72" s="3">
-        <v>2.0258333333333</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17">
-      <c r="B73" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C73" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="D73" s="3">
-        <v>8.3</v>
-      </c>
-      <c r="E73" s="3">
-        <v>5.1</v>
-      </c>
-      <c r="F73" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="G73" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H73" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I73" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J73" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K73" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L73" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M73" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="N73" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="O73" s="3">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17">
-      <c r="B89" s="3"/>
-      <c r="C89" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L89" s="3"/>
-      <c r="M89" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N89" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17">
-      <c r="B90" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C90" s="3">
-        <v>937</v>
-      </c>
-      <c r="D90" s="3">
-        <v>31</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H90" s="3">
-        <v>934</v>
-      </c>
-      <c r="I90" s="3">
-        <v>34</v>
-      </c>
-      <c r="L90" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M90" s="3">
-        <v>867</v>
-      </c>
-      <c r="N90" s="3">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="110" spans="1:17">
-      <c r="B110" s="3"/>
-      <c r="C110" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G110" s="3"/>
-      <c r="H110" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I110" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L110" s="3"/>
-      <c r="M110" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N110" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="111" spans="1:17">
-      <c r="B111" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C111" s="3">
-        <v>945</v>
-      </c>
-      <c r="D111" s="3">
-        <v>23</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H111" s="3">
-        <v>890</v>
-      </c>
-      <c r="I111" s="3">
-        <v>78</v>
-      </c>
-      <c r="L111" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M111" s="3">
-        <v>943</v>
-      </c>
-      <c r="N111" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17">
-      <c r="B131" s="3"/>
-      <c r="C131" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17">
-      <c r="B132" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C132" s="3">
-        <v>924</v>
-      </c>
-      <c r="D132" s="3">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="151" spans="1:17">
-      <c r="H151" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="153" spans="1:17">
-      <c r="B153" s="3"/>
-      <c r="C153" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17">
-      <c r="B154" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C154" s="3"/>
-      <c r="D154" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E154" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:17">
-      <c r="B155" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C155" s="3">
-        <v>0</v>
-      </c>
-      <c r="D155" s="3">
-        <v>0</v>
-      </c>
-      <c r="E155" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:17">
-      <c r="B156" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C156" s="3"/>
-      <c r="D156" s="3"/>
-      <c r="E156" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:17">
-      <c r="B157" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C157" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D157" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E157" s="3"/>
-    </row>
-    <row r="158" spans="1:17">
-      <c r="B158" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C158" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D158" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E158" s="3"/>
-    </row>
-    <row r="161" spans="1:17">
-      <c r="B161" s="3"/>
-      <c r="C161" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D161" s="3"/>
-      <c r="E161" s="3"/>
-      <c r="G161" s="3"/>
-      <c r="H161" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I161" s="3"/>
-      <c r="J161" s="3"/>
-      <c r="L161" s="3"/>
-      <c r="M161" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N161" s="3"/>
-      <c r="O161" s="3"/>
-    </row>
-    <row r="162" spans="1:17">
-      <c r="B162" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G162" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H162" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I162" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J162" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L162" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M162" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="N162" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O162" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="163" spans="1:17">
-      <c r="B163" s="3">
-        <v>198</v>
-      </c>
-      <c r="C163" s="3">
-        <v>94</v>
-      </c>
-      <c r="D163" s="3">
-        <v>0</v>
-      </c>
-      <c r="E163" s="3">
-        <v>0</v>
-      </c>
-      <c r="G163" s="3">
-        <v>182</v>
-      </c>
-      <c r="H163" s="3">
-        <v>189</v>
-      </c>
-      <c r="I163" s="3">
-        <v>0</v>
-      </c>
-      <c r="J163" s="3">
-        <v>0</v>
-      </c>
-      <c r="L163" s="3">
-        <v>380</v>
-      </c>
-      <c r="M163" s="3">
-        <v>283</v>
-      </c>
-      <c r="N163" s="3">
-        <v>0</v>
-      </c>
-      <c r="O163" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:17">
-      <c r="H181" s="10" t="s">
+    <row r="208" spans="1:17">
+      <c r="B208" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="182" spans="1:17">
-      <c r="B182" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C182" s="3"/>
-      <c r="D182" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E182" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="183" spans="1:17">
-      <c r="B183" s="3"/>
-      <c r="C183" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D183" s="3">
-        <v>1503442.66</v>
-      </c>
-      <c r="E183" s="3">
-        <v>72.02</v>
-      </c>
-    </row>
-    <row r="184" spans="1:17">
-      <c r="B184" s="3"/>
-      <c r="C184" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D184" s="3">
-        <v>375</v>
-      </c>
-      <c r="E184" s="3">
-        <v>72.12</v>
-      </c>
-    </row>
-    <row r="185" spans="1:17">
-      <c r="B185" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C185" s="3"/>
-      <c r="D185" s="3"/>
-      <c r="E185" s="3"/>
-      <c r="I185" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J185" s="3"/>
-      <c r="K185" s="3"/>
-    </row>
-    <row r="186" spans="1:17">
-      <c r="B186" s="3"/>
-      <c r="C186" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D186" s="3">
-        <v>1503443</v>
-      </c>
-      <c r="E186" s="3"/>
-      <c r="I186" s="3"/>
-      <c r="J186" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K186" s="3">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="187" spans="1:17">
-      <c r="B187" s="3"/>
-      <c r="C187" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D187" s="3"/>
-      <c r="E187" s="3"/>
-      <c r="I187" s="3"/>
-      <c r="J187" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K187" s="3"/>
-    </row>
-    <row r="207" spans="1:17">
-      <c r="B207" s="3"/>
-      <c r="C207" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D207" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E207" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F207" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G207" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H207" s="3"/>
-      <c r="I207" s="3"/>
-      <c r="J207" s="3"/>
-      <c r="K207" s="3"/>
-      <c r="L207" s="3"/>
-      <c r="M207" s="3"/>
-      <c r="N207" s="3"/>
-      <c r="O207" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="208" spans="1:17">
-      <c r="B208" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C208" s="3">
-        <v>143</v>
-      </c>
-      <c r="D208" s="3">
-        <v>213</v>
-      </c>
-      <c r="E208" s="3">
-        <v>226</v>
-      </c>
-      <c r="F208" s="3">
-        <v>51</v>
-      </c>
-      <c r="G208" s="3">
-        <v>1</v>
-      </c>
-      <c r="H208" s="3"/>
-      <c r="I208" s="3"/>
-      <c r="J208" s="3"/>
-      <c r="K208" s="3"/>
-      <c r="L208" s="3"/>
-      <c r="M208" s="3"/>
-      <c r="N208" s="3"/>
-      <c r="O208" s="3">
+      <c r="C208">
+        <v>131</v>
+      </c>
+      <c r="D208">
+        <v>174</v>
+      </c>
+      <c r="E208">
+        <v>223</v>
+      </c>
+      <c r="F208">
+        <v>161</v>
+      </c>
+      <c r="G208">
+        <v>171</v>
+      </c>
+      <c r="H208">
+        <v>249</v>
+      </c>
+      <c r="I208">
+        <v>204</v>
+      </c>
+      <c r="J208">
+        <v>115</v>
+      </c>
+      <c r="K208">
+        <v>167</v>
+      </c>
+      <c r="L208">
+        <v>269</v>
+      </c>
+      <c r="M208">
+        <v>199</v>
+      </c>
+      <c r="N208">
+        <v>251</v>
+      </c>
+      <c r="O208">
         <f>SUM(C208:N208)</f>
-        <v>634</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="209" spans="1:17">
-      <c r="B209" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C209" s="3">
-        <v>73.2394</v>
-      </c>
-      <c r="D209" s="3">
-        <v>74.5665</v>
-      </c>
-      <c r="E209" s="3">
-        <v>69.0909</v>
-      </c>
-      <c r="F209" s="3">
-        <v>66.6667</v>
-      </c>
-      <c r="G209" s="3"/>
-      <c r="H209" s="3"/>
-      <c r="I209" s="3"/>
-      <c r="J209" s="3"/>
-      <c r="K209" s="3"/>
-      <c r="L209" s="3"/>
-      <c r="M209" s="3"/>
-      <c r="N209" s="3"/>
-      <c r="O209" s="3">
+      <c r="B209" t="s">
+        <v>77</v>
+      </c>
+      <c r="C209">
+        <v>75.0</v>
+      </c>
+      <c r="D209">
+        <v>73.2919</v>
+      </c>
+      <c r="E209">
+        <v>71.3636</v>
+      </c>
+      <c r="F209">
+        <v>77.6923</v>
+      </c>
+      <c r="G209">
+        <v>82.2222</v>
+      </c>
+      <c r="H209">
+        <v>79.0476</v>
+      </c>
+      <c r="I209">
+        <v>69.7802</v>
+      </c>
+      <c r="J209">
+        <v>72.9412</v>
+      </c>
+      <c r="K209">
+        <v>76.0331</v>
+      </c>
+      <c r="L209">
+        <v>77.1552</v>
+      </c>
+      <c r="M209">
+        <v>70.6587</v>
+      </c>
+      <c r="N209">
+        <v>78.6458</v>
+      </c>
+      <c r="O209">
         <f>SUM(C209:N209) / 12</f>
-        <v>23.630291666667</v>
+        <v>75.319316666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout sécurité dans la création du fichier excel volval pour les achats en dessous de 2K, verification de la présence des données
</commit_message>
<xml_diff>
--- a/public/nom_de_fichier.xlsx
+++ b/public/nom_de_fichier.xlsx
@@ -92,28 +92,28 @@
     <t>Délai</t>
   </si>
   <si>
-    <t>&gt; 3j / 8.33%</t>
-  </si>
-  <si>
-    <t>&gt; 3j / 58.33%</t>
-  </si>
-  <si>
-    <t>&gt; 7j / 41.67%</t>
-  </si>
-  <si>
-    <t>&gt; à 15j / 75.00%</t>
-  </si>
-  <si>
-    <t>&lt;= 3j / 91.67%</t>
-  </si>
-  <si>
-    <t>&lt;= 3j / 41.67%</t>
-  </si>
-  <si>
-    <t>&lt;= 7j / 58.33%</t>
-  </si>
-  <si>
-    <t>&lt;= 15j / 25.00%</t>
+    <t>&gt; 3j / 20.28%</t>
+  </si>
+  <si>
+    <t>&gt; 3j / 71.09%</t>
+  </si>
+  <si>
+    <t>&gt; 7j / 10.11%</t>
+  </si>
+  <si>
+    <t>&gt; à 15j / 24.78%</t>
+  </si>
+  <si>
+    <t>&lt;= 3j / 79.72%</t>
+  </si>
+  <si>
+    <t>&lt;= 3j / 28.91%</t>
+  </si>
+  <si>
+    <t>&lt;= 7j / 89.89%</t>
+  </si>
+  <si>
+    <t>&lt;= 15j / 75.22%</t>
   </si>
   <si>
     <t>Transmissions</t>
@@ -471,40 +471,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,40 +534,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,40 +597,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>134</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>231</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>151</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>170</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>93</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>141</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>230</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>206</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>151</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,40 +660,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>127</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>146</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -855,7 +855,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24119</c:v>
+                  <c:v>7014508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -864,6 +864,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$E$147</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -871,6 +882,12 @@
           <c:val>
             <c:numRef>
               <c:f>Worksheet!$E$146</c:f>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>31561</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1068,7 +1085,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1077,6 +1094,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$L$147</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -1084,6 +1112,12 @@
           <c:val>
             <c:numRef>
               <c:f>Worksheet!$L$146</c:f>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -1279,31 +1313,31 @@
                   <c:v>Mars</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>Avril</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>Mai</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>Juin</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>Juillet</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>Août</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>Septembre</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>Octobre</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>Novembre</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>Décembre</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1314,40 +1348,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1537,40 +1571,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3427042.87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6560707.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>15062208.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>17140160.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>20053863.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>26269693.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>32591922.51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>34953853.13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38002</c:v>
+                  <c:v>41459928.74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38002</c:v>
+                  <c:v>45792861</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38002</c:v>
+                  <c:v>49071173.51</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38002</c:v>
+                  <c:v>61969650.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1599,40 +1633,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3427042.87</c:v>
+                  <c:v>1321328.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6560707.63</c:v>
+                  <c:v>3408628.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15062208.99</c:v>
+                  <c:v>5913110.07</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17140160.68</c:v>
+                  <c:v>7607418.46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20053863.04</c:v>
+                  <c:v>10888571.71</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26269693.94</c:v>
+                  <c:v>14512085.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32591922.51</c:v>
+                  <c:v>25615021.51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34953853.13</c:v>
+                  <c:v>28223412.06</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41459928.74</c:v>
+                  <c:v>31072730.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45792861</c:v>
+                  <c:v>34100831.32</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49071173.51</c:v>
+                  <c:v>38781150.42</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61969650.7</c:v>
+                  <c:v>42881828.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1769,10 +1803,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 3j / 91.67%</c:v>
+                  <c:v>&lt;= 3j / 79.72%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; 3j / 8.33%</c:v>
+                  <c:v>&gt; 3j / 20.28%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1783,10 +1817,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>2658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1883,10 +1917,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 3j / 41.67%</c:v>
+                  <c:v>&lt;= 3j / 28.91%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; 3j / 58.33%</c:v>
+                  <c:v>&gt; 3j / 71.09%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1897,10 +1931,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>964</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>2370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1997,10 +2031,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 7j / 58.33%</c:v>
+                  <c:v>&lt;= 7j / 89.89%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; 7j / 41.67%</c:v>
+                  <c:v>&gt; 7j / 10.11%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2011,10 +2045,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>2997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2111,10 +2145,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>&lt;= 15j / 25.00%</c:v>
+                  <c:v>&lt;= 15j / 75.22%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; à 15j / 75.00%</c:v>
+                  <c:v>&gt; à 15j / 24.78%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2125,10 +2159,10 @@
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2508</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2256,10 +2290,10 @@
               <c:numCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>693</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>616</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2393,10 +2427,10 @@
               <c:numCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>644</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2524,10 +2558,10 @@
               <c:numCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>1337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>881</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3338,44 +3372,44 @@
         <v>2</v>
       </c>
       <c r="C4" s="3">
-        <v>0.0</v>
+        <v>134.0</v>
       </c>
       <c r="D4" s="3">
-        <v>0.0</v>
+        <v>160.0</v>
       </c>
       <c r="E4" s="3">
-        <v>0.0</v>
+        <v>231.0</v>
       </c>
       <c r="F4" s="3">
-        <v>0.0</v>
+        <v>125.0</v>
       </c>
       <c r="G4" s="3">
-        <v>0.0</v>
+        <v>151.0</v>
       </c>
       <c r="H4" s="3">
-        <v>0.0</v>
+        <v>212.0</v>
       </c>
       <c r="I4" s="3">
-        <v>0.0</v>
+        <v>170.0</v>
       </c>
       <c r="J4" s="3">
-        <v>0.0</v>
+        <v>93.0</v>
       </c>
       <c r="K4" s="3">
-        <v>0.0</v>
+        <v>141.0</v>
       </c>
       <c r="L4" s="3">
-        <v>0.0</v>
+        <v>230.0</v>
       </c>
       <c r="M4" s="3">
-        <v>0.0</v>
+        <v>206.0</v>
       </c>
       <c r="N4" s="3">
-        <v>0.0</v>
+        <v>151.0</v>
       </c>
       <c r="O4" s="2">
         <f>SUM(C4:N4)</f>
-        <v>0</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -3383,44 +3417,44 @@
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <v>0.0</v>
+        <v>103.0</v>
       </c>
       <c r="D5" s="4">
-        <v>0.0</v>
+        <v>116.0</v>
       </c>
       <c r="E5" s="4">
-        <v>0.0</v>
+        <v>138.0</v>
       </c>
       <c r="F5" s="4">
-        <v>0.0</v>
+        <v>103.0</v>
       </c>
       <c r="G5" s="4">
-        <v>0.0</v>
+        <v>131.0</v>
       </c>
       <c r="H5" s="4">
-        <v>0.0</v>
+        <v>117.0</v>
       </c>
       <c r="I5" s="4">
-        <v>0.0</v>
+        <v>124.0</v>
       </c>
       <c r="J5" s="4">
-        <v>0.0</v>
+        <v>99.0</v>
       </c>
       <c r="K5" s="4">
-        <v>2.0</v>
+        <v>112.0</v>
       </c>
       <c r="L5" s="4">
-        <v>0.0</v>
+        <v>127.0</v>
       </c>
       <c r="M5" s="4">
-        <v>0.0</v>
+        <v>146.0</v>
       </c>
       <c r="N5" s="4">
-        <v>0.0</v>
+        <v>130.0</v>
       </c>
       <c r="O5" s="2">
         <f>SUM(C5:N5)</f>
-        <v>2</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -3428,44 +3462,44 @@
         <v>4</v>
       </c>
       <c r="C6" s="5">
-        <v>0.0</v>
+        <v>237.0</v>
       </c>
       <c r="D6" s="5">
-        <v>0.0</v>
+        <v>276.0</v>
       </c>
       <c r="E6" s="5">
-        <v>0.0</v>
+        <v>369.0</v>
       </c>
       <c r="F6" s="5">
-        <v>0.0</v>
+        <v>228.0</v>
       </c>
       <c r="G6" s="5">
-        <v>0.0</v>
+        <v>282.0</v>
       </c>
       <c r="H6" s="5">
-        <v>0.0</v>
+        <v>329.0</v>
       </c>
       <c r="I6" s="5">
-        <v>0.0</v>
+        <v>294.0</v>
       </c>
       <c r="J6" s="5">
-        <v>0.0</v>
+        <v>192.0</v>
       </c>
       <c r="K6" s="5">
-        <v>2.0</v>
+        <v>253.0</v>
       </c>
       <c r="L6" s="5">
-        <v>0.0</v>
+        <v>357.0</v>
       </c>
       <c r="M6" s="5">
-        <v>0.0</v>
+        <v>352.0</v>
       </c>
       <c r="N6" s="5">
-        <v>0.0</v>
+        <v>281.0</v>
       </c>
       <c r="O6" s="2">
         <f>SUM(C6:N6)</f>
-        <v>2</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -3473,44 +3507,44 @@
         <v>20</v>
       </c>
       <c r="C7" s="6">
-        <v>134.0</v>
+        <v>120.0</v>
       </c>
       <c r="D7" s="6">
+        <v>138.0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>236.0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>205.0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>227.0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>206.0</v>
+      </c>
+      <c r="I7" s="6">
         <v>160.0</v>
       </c>
-      <c r="E7" s="6">
-        <v>231.0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>125.0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>151.0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>212.0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>170.0</v>
-      </c>
       <c r="J7" s="6">
-        <v>93.0</v>
+        <v>99.0</v>
       </c>
       <c r="K7" s="6">
-        <v>141.0</v>
+        <v>159.0</v>
       </c>
       <c r="L7" s="6">
-        <v>230.0</v>
+        <v>215.0</v>
       </c>
       <c r="M7" s="6">
-        <v>206.0</v>
+        <v>208.0</v>
       </c>
       <c r="N7" s="6">
-        <v>151.0</v>
+        <v>210.0</v>
       </c>
       <c r="O7">
         <f>SUM(C7:N7)</f>
-        <v>2004</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -3518,44 +3552,44 @@
         <v>21</v>
       </c>
       <c r="C8" s="7">
+        <v>107.0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>105.0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>152.0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>104.0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>192.0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>148.0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>102.0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>174.0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>139.0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>134.0</v>
+      </c>
+      <c r="N8" s="7">
         <v>103.0</v>
-      </c>
-      <c r="D8" s="7">
-        <v>116.0</v>
-      </c>
-      <c r="E8" s="7">
-        <v>138.0</v>
-      </c>
-      <c r="F8" s="7">
-        <v>103.0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>131.0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>117.0</v>
-      </c>
-      <c r="I8" s="7">
-        <v>124.0</v>
-      </c>
-      <c r="J8" s="7">
-        <v>99.0</v>
-      </c>
-      <c r="K8" s="7">
-        <v>112.0</v>
-      </c>
-      <c r="L8" s="7">
-        <v>127.0</v>
-      </c>
-      <c r="M8" s="7">
-        <v>146.0</v>
-      </c>
-      <c r="N8" s="7">
-        <v>130.0</v>
       </c>
       <c r="O8">
         <f>SUM(C8:N8)</f>
-        <v>1446</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -3563,44 +3597,44 @@
         <v>22</v>
       </c>
       <c r="C9" s="8">
-        <v>237.0</v>
+        <v>227.0</v>
       </c>
       <c r="D9" s="8">
-        <v>276.0</v>
+        <v>243.0</v>
       </c>
       <c r="E9" s="8">
-        <v>369.0</v>
+        <v>388.0</v>
       </c>
       <c r="F9" s="8">
-        <v>228.0</v>
+        <v>309.0</v>
       </c>
       <c r="G9" s="8">
-        <v>282.0</v>
+        <v>419.0</v>
       </c>
       <c r="H9" s="8">
-        <v>329.0</v>
+        <v>354.0</v>
       </c>
       <c r="I9" s="8">
-        <v>294.0</v>
+        <v>262.0</v>
       </c>
       <c r="J9" s="8">
-        <v>192.0</v>
+        <v>176.0</v>
       </c>
       <c r="K9" s="8">
-        <v>253.0</v>
+        <v>333.0</v>
       </c>
       <c r="L9" s="8">
-        <v>357.0</v>
+        <v>354.0</v>
       </c>
       <c r="M9" s="8">
-        <v>352.0</v>
+        <v>342.0</v>
       </c>
       <c r="N9" s="8">
-        <v>281.0</v>
+        <v>313.0</v>
       </c>
       <c r="O9">
         <f>SUM(C9:N9)</f>
-        <v>3450</v>
+        <v>3720</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -3652,44 +3686,44 @@
         <v>2</v>
       </c>
       <c r="C12" s="3">
-        <v>0.0</v>
+        <v>573434.82</v>
       </c>
       <c r="D12" s="3">
-        <v>0.0</v>
+        <v>745787.03</v>
       </c>
       <c r="E12" s="3">
-        <v>0.0</v>
+        <v>1017141.82</v>
       </c>
       <c r="F12" s="3">
-        <v>0.0</v>
+        <v>563515.61</v>
       </c>
       <c r="G12" s="3">
-        <v>0.0</v>
+        <v>809312.02</v>
       </c>
       <c r="H12" s="3">
-        <v>0.0</v>
+        <v>804991.44</v>
       </c>
       <c r="I12" s="3">
-        <v>0.0</v>
+        <v>1430406.73</v>
       </c>
       <c r="J12" s="3">
-        <v>0.0</v>
+        <v>396459.44</v>
       </c>
       <c r="K12" s="3">
-        <v>0.0</v>
+        <v>729066.96</v>
       </c>
       <c r="L12" s="3">
-        <v>0.0</v>
+        <v>1531842.53</v>
       </c>
       <c r="M12" s="3">
-        <v>0.0</v>
+        <v>1089886.45</v>
       </c>
       <c r="N12" s="3">
-        <v>0.0</v>
+        <v>1029487.17</v>
       </c>
       <c r="O12" s="2">
         <f>SUM(C12:N12)</f>
-        <v>0</v>
+        <v>10721332.02</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -3697,44 +3731,44 @@
         <v>3</v>
       </c>
       <c r="C13" s="4">
-        <v>0.0</v>
+        <v>2853608.05</v>
       </c>
       <c r="D13" s="4">
-        <v>0.0</v>
+        <v>2387877.73</v>
       </c>
       <c r="E13" s="4">
-        <v>0.0</v>
+        <v>7484359.54</v>
       </c>
       <c r="F13" s="4">
-        <v>0.0</v>
+        <v>1514436.08</v>
       </c>
       <c r="G13" s="4">
-        <v>0.0</v>
+        <v>2104390.34</v>
       </c>
       <c r="H13" s="4">
-        <v>0.0</v>
+        <v>5410839.46</v>
       </c>
       <c r="I13" s="4">
-        <v>0.0</v>
+        <v>4891821.84</v>
       </c>
       <c r="J13" s="4">
-        <v>0.0</v>
+        <v>1965471.18</v>
       </c>
       <c r="K13" s="4">
-        <v>38002.0</v>
+        <v>5777008.65</v>
       </c>
       <c r="L13" s="4">
-        <v>0.0</v>
+        <v>2801089.73</v>
       </c>
       <c r="M13" s="4">
-        <v>0.0</v>
+        <v>2188426.06</v>
       </c>
       <c r="N13" s="4">
-        <v>0.0</v>
+        <v>11868990.02</v>
       </c>
       <c r="O13" s="2">
         <f>SUM(C13:N13)</f>
-        <v>38002</v>
+        <v>51248318.68</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -3742,44 +3776,44 @@
         <v>4</v>
       </c>
       <c r="C14" s="5">
-        <v>0.0</v>
+        <v>3427042.87</v>
       </c>
       <c r="D14" s="5">
-        <v>0.0</v>
+        <v>6560707.63</v>
       </c>
       <c r="E14" s="5">
-        <v>0.0</v>
+        <v>15062208.99</v>
       </c>
       <c r="F14" s="5">
-        <v>0.0</v>
+        <v>17140160.68</v>
       </c>
       <c r="G14" s="5">
-        <v>0.0</v>
+        <v>20053863.04</v>
       </c>
       <c r="H14" s="5">
-        <v>0.0</v>
+        <v>26269693.94</v>
       </c>
       <c r="I14" s="5">
-        <v>0.0</v>
+        <v>32591922.51</v>
       </c>
       <c r="J14" s="5">
-        <v>0.0</v>
+        <v>34953853.13</v>
       </c>
       <c r="K14" s="5">
-        <v>38002.0</v>
+        <v>41459928.74</v>
       </c>
       <c r="L14" s="5">
-        <v>38002.0</v>
+        <v>45792861.0</v>
       </c>
       <c r="M14" s="5">
-        <v>38002.0</v>
+        <v>49071173.51</v>
       </c>
       <c r="N14" s="5">
-        <v>38002.0</v>
+        <v>61969650.7</v>
       </c>
       <c r="O14" s="2">
         <f>SUM(C14:N14)</f>
-        <v>152008</v>
+        <v>354353066.74</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -3787,44 +3821,44 @@
         <v>20</v>
       </c>
       <c r="C15" s="6">
-        <v>573434.82</v>
+        <v>312452.75</v>
       </c>
       <c r="D15" s="6">
-        <v>745787.03</v>
+        <v>557343.77</v>
       </c>
       <c r="E15" s="6">
-        <v>1017141.82</v>
+        <v>982521.22</v>
       </c>
       <c r="F15" s="6">
-        <v>563515.61</v>
+        <v>842191.86</v>
       </c>
       <c r="G15" s="6">
-        <v>809312.02</v>
+        <v>729838.13</v>
       </c>
       <c r="H15" s="6">
-        <v>804991.44</v>
+        <v>1035253.76</v>
       </c>
       <c r="I15" s="6">
-        <v>1430406.73</v>
+        <v>726859.11</v>
       </c>
       <c r="J15" s="6">
-        <v>396459.44</v>
+        <v>452202.63</v>
       </c>
       <c r="K15" s="6">
-        <v>729066.96</v>
+        <v>618165.94</v>
       </c>
       <c r="L15" s="6">
-        <v>1531842.53</v>
+        <v>1062671.69</v>
       </c>
       <c r="M15" s="6">
-        <v>1089886.45</v>
+        <v>822340.52</v>
       </c>
       <c r="N15" s="6">
-        <v>1029487.17</v>
+        <v>1187753.03</v>
       </c>
       <c r="O15">
         <f>SUM(C15:N15)</f>
-        <v>10721332.02</v>
+        <v>9329594.41</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -3832,44 +3866,44 @@
         <v>21</v>
       </c>
       <c r="C16" s="7">
-        <v>2853608.05</v>
+        <v>1008875.94</v>
       </c>
       <c r="D16" s="7">
-        <v>2387877.73</v>
+        <v>1529955.59</v>
       </c>
       <c r="E16" s="7">
-        <v>7484359.54</v>
+        <v>1521960.8</v>
       </c>
       <c r="F16" s="7">
-        <v>1514436.08</v>
+        <v>852116.53</v>
       </c>
       <c r="G16" s="7">
-        <v>2104390.34</v>
+        <v>2551315.12</v>
       </c>
       <c r="H16" s="7">
-        <v>5410839.46</v>
+        <v>2588259.65</v>
       </c>
       <c r="I16" s="7">
-        <v>4891821.84</v>
+        <v>10376077.28</v>
       </c>
       <c r="J16" s="7">
-        <v>1965471.18</v>
+        <v>2156187.92</v>
       </c>
       <c r="K16" s="7">
-        <v>5777008.65</v>
+        <v>2231152.02</v>
       </c>
       <c r="L16" s="7">
-        <v>2801089.73</v>
+        <v>1965429.61</v>
       </c>
       <c r="M16" s="7">
-        <v>2188426.06</v>
+        <v>3857978.58</v>
       </c>
       <c r="N16" s="7">
-        <v>11868990.02</v>
+        <v>2912924.86</v>
       </c>
       <c r="O16">
         <f>SUM(C16:N16)</f>
-        <v>51248318.68</v>
+        <v>33552233.9</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -3877,62 +3911,86 @@
         <v>22</v>
       </c>
       <c r="C17" s="8">
-        <v>3427042.87</v>
+        <v>1321328.69</v>
       </c>
       <c r="D17" s="8">
-        <v>6560707.63</v>
+        <v>3408628.05</v>
       </c>
       <c r="E17" s="8">
-        <v>15062208.99</v>
+        <v>5913110.07</v>
       </c>
       <c r="F17" s="8">
-        <v>17140160.68</v>
+        <v>7607418.46</v>
       </c>
       <c r="G17" s="8">
-        <v>20053863.04</v>
+        <v>10888571.71</v>
       </c>
       <c r="H17" s="8">
-        <v>26269693.94</v>
+        <v>14512085.12</v>
       </c>
       <c r="I17" s="8">
-        <v>32591922.51</v>
+        <v>25615021.51</v>
       </c>
       <c r="J17" s="8">
-        <v>34953853.13</v>
+        <v>28223412.06</v>
       </c>
       <c r="K17" s="8">
-        <v>41459928.74</v>
+        <v>31072730.02</v>
       </c>
       <c r="L17" s="8">
-        <v>45792861.0</v>
+        <v>34100831.32</v>
       </c>
       <c r="M17" s="8">
-        <v>49071173.51</v>
+        <v>38781150.42</v>
       </c>
       <c r="N17" s="8">
-        <v>61969650.7</v>
+        <v>42881828.31</v>
       </c>
       <c r="O17">
         <f>SUM(C17:N17)</f>
-        <v>354353066.74</v>
+        <v>244326115.74</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="O18" s="2" t="s">
         <v>17</v>
       </c>
@@ -3941,63 +3999,135 @@
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="C19" s="3">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3">
+        <v>59</v>
+      </c>
+      <c r="E19" s="3">
+        <v>82</v>
+      </c>
+      <c r="F19" s="3">
+        <v>45</v>
+      </c>
+      <c r="G19" s="3">
+        <v>67</v>
+      </c>
+      <c r="H19" s="3">
+        <v>100</v>
+      </c>
+      <c r="I19" s="3">
+        <v>56</v>
+      </c>
+      <c r="J19" s="3">
+        <v>41</v>
+      </c>
+      <c r="K19" s="3">
+        <v>45</v>
+      </c>
+      <c r="L19" s="3">
+        <v>79</v>
+      </c>
+      <c r="M19" s="3">
+        <v>59</v>
+      </c>
+      <c r="N19" s="3">
+        <v>45</v>
+      </c>
       <c r="O19" s="2">
         <f>SUM(C19:N19)</f>
-        <v>0</v>
+        <v>741</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
+      <c r="C20" s="4">
+        <v>46</v>
+      </c>
+      <c r="D20" s="4">
+        <v>52</v>
+      </c>
+      <c r="E20" s="4">
+        <v>78</v>
+      </c>
+      <c r="F20" s="4">
+        <v>46</v>
+      </c>
+      <c r="G20" s="4">
+        <v>56</v>
+      </c>
+      <c r="H20" s="4">
+        <v>58</v>
+      </c>
+      <c r="I20" s="4">
+        <v>46</v>
+      </c>
+      <c r="J20" s="4">
+        <v>42</v>
+      </c>
+      <c r="K20" s="4">
+        <v>60</v>
+      </c>
+      <c r="L20" s="4">
+        <v>73</v>
+      </c>
+      <c r="M20" s="4">
+        <v>71</v>
+      </c>
+      <c r="N20" s="4">
+        <v>53</v>
+      </c>
       <c r="O20" s="2">
         <f>SUM(C20:N20)</f>
-        <v>0</v>
+        <v>681</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
+      <c r="C21" s="5">
+        <v>109</v>
+      </c>
+      <c r="D21" s="5">
+        <v>111</v>
+      </c>
+      <c r="E21" s="5">
+        <v>160</v>
+      </c>
+      <c r="F21" s="5">
+        <v>91</v>
+      </c>
+      <c r="G21" s="5">
+        <v>123</v>
+      </c>
+      <c r="H21" s="5">
+        <v>158</v>
+      </c>
+      <c r="I21" s="5">
+        <v>102</v>
+      </c>
+      <c r="J21" s="5">
+        <v>83</v>
+      </c>
+      <c r="K21" s="5">
+        <v>105</v>
+      </c>
+      <c r="L21" s="5">
+        <v>152</v>
+      </c>
+      <c r="M21" s="5">
+        <v>130</v>
+      </c>
+      <c r="N21" s="5">
+        <v>98</v>
+      </c>
       <c r="O21" s="2">
         <f>SUM(C21:N21)</f>
-        <v>0</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -4005,44 +4135,44 @@
         <v>20</v>
       </c>
       <c r="C22" s="9">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="9">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E22" s="9">
+        <v>114</v>
+      </c>
+      <c r="F22" s="9">
+        <v>92</v>
+      </c>
+      <c r="G22" s="9">
+        <v>108</v>
+      </c>
+      <c r="H22" s="9">
+        <v>91</v>
+      </c>
+      <c r="I22" s="9">
+        <v>65</v>
+      </c>
+      <c r="J22" s="9">
+        <v>40</v>
+      </c>
+      <c r="K22" s="9">
+        <v>78</v>
+      </c>
+      <c r="L22" s="9">
         <v>82</v>
       </c>
-      <c r="F22" s="9">
-        <v>45</v>
-      </c>
-      <c r="G22" s="9">
-        <v>67</v>
-      </c>
-      <c r="H22" s="9">
-        <v>100</v>
-      </c>
-      <c r="I22" s="9">
-        <v>56</v>
-      </c>
-      <c r="J22" s="9">
-        <v>41</v>
-      </c>
-      <c r="K22" s="9">
-        <v>45</v>
-      </c>
-      <c r="L22" s="9">
-        <v>79</v>
-      </c>
       <c r="M22" s="9">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="N22" s="9">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="O22" s="2">
         <f>SUM(C22:N22)</f>
-        <v>741</v>
+        <v>976</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -4050,44 +4180,44 @@
         <v>21</v>
       </c>
       <c r="C23" s="10">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D23" s="10">
+        <v>50</v>
+      </c>
+      <c r="E23" s="10">
+        <v>55</v>
+      </c>
+      <c r="F23" s="10">
+        <v>60</v>
+      </c>
+      <c r="G23" s="10">
+        <v>100</v>
+      </c>
+      <c r="H23" s="10">
+        <v>86</v>
+      </c>
+      <c r="I23" s="10">
         <v>52</v>
       </c>
-      <c r="E23" s="10">
-        <v>78</v>
-      </c>
-      <c r="F23" s="10">
-        <v>46</v>
-      </c>
-      <c r="G23" s="10">
-        <v>56</v>
-      </c>
-      <c r="H23" s="10">
+      <c r="J23" s="10">
+        <v>37</v>
+      </c>
+      <c r="K23" s="10">
+        <v>107</v>
+      </c>
+      <c r="L23" s="10">
+        <v>75</v>
+      </c>
+      <c r="M23" s="10">
         <v>58</v>
       </c>
-      <c r="I23" s="10">
-        <v>46</v>
-      </c>
-      <c r="J23" s="10">
-        <v>42</v>
-      </c>
-      <c r="K23" s="10">
-        <v>60</v>
-      </c>
-      <c r="L23" s="10">
-        <v>73</v>
-      </c>
-      <c r="M23" s="10">
-        <v>71</v>
-      </c>
       <c r="N23" s="10">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="O23" s="2">
         <f>SUM(C23:N23)</f>
-        <v>681</v>
+        <v>777</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -4095,44 +4225,44 @@
         <v>22</v>
       </c>
       <c r="C24" s="11">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D24" s="11">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E24" s="11">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="F24" s="11">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="G24" s="11">
-        <v>123</v>
+        <v>208</v>
       </c>
       <c r="H24" s="11">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="I24" s="11">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="J24" s="11">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K24" s="11">
-        <v>105</v>
+        <v>185</v>
       </c>
       <c r="L24" s="11">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="M24" s="11">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="N24" s="11">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="O24" s="2">
         <f>SUM(C24:N24)</f>
-        <v>1422</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -4333,43 +4463,43 @@
         <v>33</v>
       </c>
       <c r="C69" s="13">
-        <v>2.6</v>
+        <v>3.54</v>
       </c>
       <c r="D69" s="13">
-        <v>1.0</v>
+        <v>4.76</v>
       </c>
       <c r="E69" s="13">
-        <v>0</v>
+        <v>4.7</v>
       </c>
       <c r="F69" s="13">
-        <v>0</v>
+        <v>3.05</v>
       </c>
       <c r="G69" s="13">
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="H69" s="13">
-        <v>0</v>
+        <v>3.67</v>
       </c>
       <c r="I69" s="13">
-        <v>0</v>
+        <v>2.83</v>
       </c>
       <c r="J69" s="13">
-        <v>0</v>
+        <v>1.29</v>
       </c>
       <c r="K69" s="13">
-        <v>0.0</v>
+        <v>1.42</v>
       </c>
       <c r="L69" s="13">
-        <v>0</v>
+        <v>1.39</v>
       </c>
       <c r="M69" s="13">
-        <v>0</v>
+        <v>1.62</v>
       </c>
       <c r="N69" s="13">
-        <v>0</v>
+        <v>2.27</v>
       </c>
       <c r="O69" s="13">
-        <v>0.3</v>
+        <v>3.0658333333333</v>
       </c>
     </row>
     <row r="70" spans="1:17">
@@ -4377,43 +4507,43 @@
         <v>34</v>
       </c>
       <c r="C70" s="13">
-        <v>18.0</v>
+        <v>7.74</v>
       </c>
       <c r="D70" s="13">
-        <v>54.0</v>
+        <v>6.87</v>
       </c>
       <c r="E70" s="13">
-        <v>0</v>
+        <v>8.16</v>
       </c>
       <c r="F70" s="13">
-        <v>0</v>
+        <v>7.88</v>
       </c>
       <c r="G70" s="13">
-        <v>0</v>
+        <v>12.37</v>
       </c>
       <c r="H70" s="13">
-        <v>0</v>
+        <v>7.21</v>
       </c>
       <c r="I70" s="13">
-        <v>0</v>
+        <v>6.36</v>
       </c>
       <c r="J70" s="13">
-        <v>0</v>
+        <v>7.07</v>
       </c>
       <c r="K70" s="13">
-        <v>0.0</v>
+        <v>5.38</v>
       </c>
       <c r="L70" s="13">
-        <v>0</v>
+        <v>5.63</v>
       </c>
       <c r="M70" s="13">
-        <v>0</v>
+        <v>5.83</v>
       </c>
       <c r="N70" s="13">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="O70" s="13">
-        <v>6.0</v>
+        <v>7.3083333333333</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -4421,43 +4551,43 @@
         <v>35</v>
       </c>
       <c r="C71" s="13">
-        <v>18.6</v>
+        <v>2.02</v>
       </c>
       <c r="D71" s="13">
-        <v>0.0</v>
+        <v>2.92</v>
       </c>
       <c r="E71" s="13">
-        <v>0</v>
+        <v>2.13</v>
       </c>
       <c r="F71" s="13">
-        <v>0</v>
+        <v>1.07</v>
       </c>
       <c r="G71" s="13">
-        <v>0</v>
+        <v>0.83</v>
       </c>
       <c r="H71" s="13">
-        <v>0</v>
+        <v>1.88</v>
       </c>
       <c r="I71" s="13">
-        <v>0</v>
+        <v>1.66</v>
       </c>
       <c r="J71" s="13">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K71" s="13">
-        <v>0.0</v>
+        <v>1.66</v>
       </c>
       <c r="L71" s="13">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="M71" s="13">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="N71" s="13">
-        <v>0</v>
+        <v>1.49</v>
       </c>
       <c r="O71" s="13">
-        <v>1.55</v>
+        <v>1.545</v>
       </c>
     </row>
     <row r="72" spans="1:17">
@@ -4465,43 +4595,43 @@
         <v>36</v>
       </c>
       <c r="C72" s="13">
-        <v>39.2</v>
+        <v>13.3</v>
       </c>
       <c r="D72" s="13">
-        <v>55.0</v>
+        <v>14.55</v>
       </c>
       <c r="E72" s="13">
-        <v>0.0</v>
+        <v>14.99</v>
       </c>
       <c r="F72" s="13">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="G72" s="13">
-        <v>0.0</v>
+        <v>19.45</v>
       </c>
       <c r="H72" s="13">
-        <v>0.0</v>
+        <v>12.76</v>
       </c>
       <c r="I72" s="13">
-        <v>0.0</v>
+        <v>10.85</v>
       </c>
       <c r="J72" s="13">
-        <v>0.0</v>
+        <v>8.61</v>
       </c>
       <c r="K72" s="13">
-        <v>0.0</v>
+        <v>8.46</v>
       </c>
       <c r="L72" s="13">
-        <v>0.0</v>
+        <v>8.05</v>
       </c>
       <c r="M72" s="13">
-        <v>0.0</v>
+        <v>9.05</v>
       </c>
       <c r="N72" s="13">
-        <v>0.0</v>
+        <v>10.96</v>
       </c>
       <c r="O72" s="13">
-        <v>7.85</v>
+        <v>11.919166666667</v>
       </c>
     </row>
     <row r="75" spans="1:17">
@@ -4529,28 +4659,28 @@
         <v>37</v>
       </c>
       <c r="B76" s="14">
-        <v>11</v>
+        <v>2658</v>
       </c>
       <c r="C76" s="15">
-        <v>1</v>
+        <v>676</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>34</v>
       </c>
       <c r="H76" s="14">
-        <v>5</v>
+        <v>964</v>
       </c>
       <c r="I76" s="15">
-        <v>7</v>
+        <v>2370</v>
       </c>
       <c r="M76" s="13" t="s">
         <v>38</v>
       </c>
       <c r="N76" s="14">
-        <v>7</v>
+        <v>2997</v>
       </c>
       <c r="O76" s="15">
-        <v>5</v>
+        <v>337</v>
       </c>
     </row>
     <row r="91" spans="1:17">
@@ -4572,10 +4702,10 @@
         <v>39</v>
       </c>
       <c r="B93" s="14">
-        <v>3</v>
+        <v>2508</v>
       </c>
       <c r="C93" s="15">
-        <v>9</v>
+        <v>826</v>
       </c>
     </row>
     <row r="111" spans="1:17">
@@ -4599,10 +4729,10 @@
         <v>44</v>
       </c>
       <c r="D114">
-        <v>184428.99</v>
+        <v>50084826.22</v>
       </c>
       <c r="E114">
-        <v>209650.01</v>
+        <v>60316191.86</v>
       </c>
     </row>
     <row r="115" spans="1:17">
@@ -4610,13 +4740,13 @@
         <v>45</v>
       </c>
       <c r="C115">
-        <v>6</v>
+        <v>1929</v>
       </c>
       <c r="D115">
-        <v>6</v>
+        <v>1405</v>
       </c>
       <c r="E115">
-        <v>12</v>
+        <v>3334</v>
       </c>
     </row>
     <row r="116" spans="1:17">
@@ -4624,13 +4754,13 @@
         <v>46</v>
       </c>
       <c r="C116">
-        <v>4203.5</v>
+        <v>5303.97</v>
       </c>
       <c r="D116">
-        <v>30738.17</v>
+        <v>35647.56</v>
       </c>
       <c r="E116">
-        <v>34941.67</v>
+        <v>40951.53</v>
       </c>
     </row>
     <row r="117" spans="1:17">
@@ -4638,10 +4768,10 @@
         <v>47</v>
       </c>
       <c r="C117">
-        <v>12.03</v>
+        <v>16.96</v>
       </c>
       <c r="D117">
-        <v>87.97</v>
+        <v>83.04</v>
       </c>
     </row>
     <row r="118" spans="1:17">
@@ -4649,10 +4779,10 @@
         <v>48</v>
       </c>
       <c r="C118">
-        <v>50.0</v>
+        <v>57.86</v>
       </c>
       <c r="D118">
-        <v>50.0</v>
+        <v>42.14</v>
       </c>
     </row>
     <row r="121" spans="1:17">
@@ -4706,10 +4836,10 @@
     </row>
     <row r="123" spans="1:17">
       <c r="B123">
-        <v>2</v>
+        <v>693</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>616</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -4718,10 +4848,10 @@
         <v>0</v>
       </c>
       <c r="G123">
-        <v>2</v>
+        <v>644</v>
       </c>
       <c r="H123">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="I123">
         <v>0</v>
@@ -4730,10 +4860,10 @@
         <v>0</v>
       </c>
       <c r="L123">
-        <v>4</v>
+        <v>1337</v>
       </c>
       <c r="M123">
-        <v>1</v>
+        <v>881</v>
       </c>
       <c r="N123">
         <v>0</v>
@@ -4763,10 +4893,10 @@
         <v>44</v>
       </c>
       <c r="D143">
-        <v>24119.2</v>
+        <v>7046068.58</v>
       </c>
       <c r="E143">
-        <v>95.63</v>
+        <v>68.87</v>
       </c>
     </row>
     <row r="144" spans="1:17">
@@ -4774,10 +4904,10 @@
         <v>45</v>
       </c>
       <c r="D144">
-        <v>5</v>
+        <v>1466</v>
       </c>
       <c r="E144">
-        <v>83.33</v>
+        <v>76.0</v>
       </c>
     </row>
     <row r="145" spans="1:17">
@@ -4793,13 +4923,19 @@
         <v>44</v>
       </c>
       <c r="D146">
-        <v>24119</v>
+        <v>7014508</v>
+      </c>
+      <c r="E146">
+        <v>31561</v>
       </c>
       <c r="J146" t="s">
         <v>63</v>
       </c>
       <c r="K146">
-        <v>5</v>
+        <v>1459</v>
+      </c>
+      <c r="L146">
+        <v>7</v>
       </c>
     </row>
     <row r="147" spans="1:17">
@@ -4807,10 +4943,16 @@
         <v>61</v>
       </c>
       <c r="D147"/>
+      <c r="E147">
+        <v>35</v>
+      </c>
       <c r="J147" t="s">
         <v>61</v>
       </c>
       <c r="K147"/>
+      <c r="L147">
+        <v>35</v>
+      </c>
     </row>
     <row r="151" spans="1:17">
       <c r="B151" s="2"/>
@@ -4900,6 +5042,33 @@
       <c r="E167" t="s">
         <v>7</v>
       </c>
+      <c r="F167" t="s">
+        <v>8</v>
+      </c>
+      <c r="G167" t="s">
+        <v>9</v>
+      </c>
+      <c r="H167" t="s">
+        <v>10</v>
+      </c>
+      <c r="I167" t="s">
+        <v>11</v>
+      </c>
+      <c r="J167" t="s">
+        <v>12</v>
+      </c>
+      <c r="K167" t="s">
+        <v>13</v>
+      </c>
+      <c r="L167" t="s">
+        <v>14</v>
+      </c>
+      <c r="M167" t="s">
+        <v>15</v>
+      </c>
+      <c r="N167" t="s">
+        <v>16</v>
+      </c>
       <c r="O167" t="s">
         <v>17</v>
       </c>
@@ -4909,17 +5078,44 @@
         <v>64</v>
       </c>
       <c r="C168">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="D168">
-        <v>1</v>
+        <v>174</v>
       </c>
       <c r="E168">
-        <v>1</v>
+        <v>223</v>
+      </c>
+      <c r="F168">
+        <v>161</v>
+      </c>
+      <c r="G168">
+        <v>171</v>
+      </c>
+      <c r="H168">
+        <v>249</v>
+      </c>
+      <c r="I168">
+        <v>204</v>
+      </c>
+      <c r="J168">
+        <v>115</v>
+      </c>
+      <c r="K168">
+        <v>167</v>
+      </c>
+      <c r="L168">
+        <v>269</v>
+      </c>
+      <c r="M168">
+        <v>199</v>
+      </c>
+      <c r="N168">
+        <v>251</v>
       </c>
       <c r="O168">
         <f>SUM(C168:N168)</f>
-        <v>11</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="169" spans="1:17">
@@ -4927,13 +5123,44 @@
         <v>65</v>
       </c>
       <c r="C169">
-        <v>83.3333</v>
-      </c>
-      <c r="D169"/>
-      <c r="E169"/>
+        <v>75.0</v>
+      </c>
+      <c r="D169">
+        <v>73.2919</v>
+      </c>
+      <c r="E169">
+        <v>71.3636</v>
+      </c>
+      <c r="F169">
+        <v>77.6923</v>
+      </c>
+      <c r="G169">
+        <v>82.2222</v>
+      </c>
+      <c r="H169">
+        <v>79.0476</v>
+      </c>
+      <c r="I169">
+        <v>69.7802</v>
+      </c>
+      <c r="J169">
+        <v>72.9412</v>
+      </c>
+      <c r="K169">
+        <v>76.0331</v>
+      </c>
+      <c r="L169">
+        <v>77.1552</v>
+      </c>
+      <c r="M169">
+        <v>70.6587</v>
+      </c>
+      <c r="N169">
+        <v>78.6458</v>
+      </c>
       <c r="O169">
         <f>SUM(C169:N169) / 12</f>
-        <v>6.9444416666667</v>
+        <v>75.319316666667</v>
       </c>
     </row>
     <row r="180" spans="1:17">

</xml_diff>

<commit_message>
correction de bug d'affichage
</commit_message>
<xml_diff>
--- a/public/nom_de_fichier.xlsx
+++ b/public/nom_de_fichier.xlsx
@@ -86,6 +86,78 @@
     <t>TOTAL (Année Précédente)</t>
   </si>
   <si>
+    <t>VALEUR</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>MOYENNE</t>
+  </si>
+  <si>
+    <t>% VALEUR</t>
+  </si>
+  <si>
+    <t>% VOLUME</t>
+  </si>
+  <si>
+    <t>MPPA</t>
+  </si>
+  <si>
+    <t>MABC</t>
+  </si>
+  <si>
+    <t>TOTAUX</t>
+  </si>
+  <si>
+    <t>X &lt;= 1500</t>
+  </si>
+  <si>
+    <t>Montant des MPPA</t>
+  </si>
+  <si>
+    <t>1500 &lt; X &lt;=4000</t>
+  </si>
+  <si>
+    <t>4000 &lt; X &lt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X &gt; </t>
+  </si>
+  <si>
+    <t>Montant des MABC</t>
+  </si>
+  <si>
+    <t>Montant des MABC + MPPA</t>
+  </si>
+  <si>
+    <t>MPPA PME</t>
+  </si>
+  <si>
+    <t>TOP PME VALEUR</t>
+  </si>
+  <si>
+    <t>PME</t>
+  </si>
+  <si>
+    <t>DEPARTEMENT</t>
+  </si>
+  <si>
+    <t>% PME</t>
+  </si>
+  <si>
+    <t>TOP PME VOLUME</t>
+  </si>
+  <si>
+    <t>VOLUME</t>
+  </si>
+  <si>
+    <t>NB MPPA PME</t>
+  </si>
+  <si>
+    <t>% MPPA</t>
+  </si>
+  <si>
     <t>Délai d'activité annuelle</t>
   </si>
   <si>
@@ -140,79 +212,7 @@
     <t>Activités par type de marché</t>
   </si>
   <si>
-    <t>MPPA</t>
-  </si>
-  <si>
-    <t>MABC</t>
-  </si>
-  <si>
-    <t>TOTAUX</t>
-  </si>
-  <si>
-    <t>VALEUR</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>MOYENNE</t>
-  </si>
-  <si>
-    <t>% VALEUR</t>
-  </si>
-  <si>
-    <t>% VOLUME</t>
-  </si>
-  <si>
-    <t>Montant des MPPA</t>
-  </si>
-  <si>
-    <t>X &lt;= 1500</t>
-  </si>
-  <si>
-    <t>1500 &lt; X &lt;=4000</t>
-  </si>
-  <si>
-    <t>4000 &lt; X &lt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X &gt; </t>
-  </si>
-  <si>
-    <t>Montant des MABC</t>
-  </si>
-  <si>
-    <t>Montant des MABC + MPPA</t>
-  </si>
-  <si>
     <t>Activités des PME</t>
-  </si>
-  <si>
-    <t>MPPA PME</t>
-  </si>
-  <si>
-    <t>PME</t>
-  </si>
-  <si>
-    <t>% PME</t>
-  </si>
-  <si>
-    <t>TOP PME VALEUR</t>
-  </si>
-  <si>
-    <t>DEPARTEMENT</t>
-  </si>
-  <si>
-    <t>TOP PME VOLUME</t>
-  </si>
-  <si>
-    <t>VOLUME</t>
-  </si>
-  <si>
-    <t>NB MPPA PME</t>
-  </si>
-  <si>
-    <t>% MPPA</t>
   </si>
 </sst>
 </file>
@@ -1124,6 +1124,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$M$147</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -1131,12 +1142,29 @@
           <c:val>
             <c:numRef>
               <c:f>Worksheet!$M$146</c:f>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$N$147</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -1144,12 +1172,29 @@
           <c:val>
             <c:numRef>
               <c:f>Worksheet!$N$146</c:f>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$O$147</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln/>
           </c:spPr>
@@ -1157,6 +1202,12 @@
           <c:val>
             <c:numRef>
               <c:f>Worksheet!$O$146</c:f>
+              <c:numCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
@@ -4027,7 +4078,7 @@
         <v>45</v>
       </c>
       <c r="L19" s="3">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M19" s="3">
         <v>59</v>
@@ -4037,7 +4088,7 @@
       </c>
       <c r="O19" s="2">
         <f>SUM(C19:N19)</f>
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -4117,7 +4168,7 @@
         <v>105</v>
       </c>
       <c r="L21" s="5">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M21" s="5">
         <v>130</v>
@@ -4127,7 +4178,7 @@
       </c>
       <c r="O21" s="2">
         <f>SUM(C21:N21)</f>
-        <v>1422</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -4411,12 +4462,12 @@
     </row>
     <row r="67" spans="1:17">
       <c r="H67" s="12" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:17">
       <c r="B68" s="13" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>5</v>
@@ -4460,7 +4511,7 @@
     </row>
     <row r="69" spans="1:17">
       <c r="B69" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C69" s="13">
         <v>3.54</v>
@@ -4504,7 +4555,7 @@
     </row>
     <row r="70" spans="1:17">
       <c r="B70" s="13" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C70" s="13">
         <v>7.74</v>
@@ -4548,7 +4599,7 @@
     </row>
     <row r="71" spans="1:17">
       <c r="B71" s="13" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C71" s="13">
         <v>2.02</v>
@@ -4592,7 +4643,7 @@
     </row>
     <row r="72" spans="1:17">
       <c r="B72" s="13" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C72" s="13">
         <v>13.3</v>
@@ -4636,27 +4687,27 @@
     </row>
     <row r="75" spans="1:17">
       <c r="B75" s="14" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="I75" s="15" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="N75" s="14" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="O75" s="15" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:17">
       <c r="A76" s="13" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B76" s="14">
         <v>2658</v>
@@ -4665,7 +4716,7 @@
         <v>676</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="H76" s="14">
         <v>964</v>
@@ -4674,7 +4725,7 @@
         <v>2370</v>
       </c>
       <c r="M76" s="13" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="N76" s="14">
         <v>2997</v>
@@ -4689,17 +4740,17 @@
     </row>
     <row r="92" spans="1:17">
       <c r="B92" s="14" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="N92" s="13"/>
       <c r="O92" s="13"/>
     </row>
     <row r="93" spans="1:17">
       <c r="A93" s="13" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B93" s="14">
         <v>2508</v>
@@ -4710,249 +4761,284 @@
     </row>
     <row r="111" spans="1:17">
       <c r="H111" s="12" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="113" spans="1:17">
-      <c r="C113" t="s">
-        <v>41</v>
-      </c>
-      <c r="D113" t="s">
-        <v>42</v>
-      </c>
-      <c r="E113" t="s">
-        <v>43</v>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="114" spans="1:17">
-      <c r="B114" t="s">
-        <v>44</v>
-      </c>
-      <c r="D114">
+      <c r="B114" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2">
         <v>50084826.22</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="2">
         <v>60316191.86</v>
       </c>
     </row>
     <row r="115" spans="1:17">
-      <c r="B115" t="s">
-        <v>45</v>
-      </c>
-      <c r="C115">
+      <c r="B115" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C115" s="2">
         <v>1929</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="2">
         <v>1405</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="2">
         <v>3334</v>
       </c>
     </row>
     <row r="116" spans="1:17">
-      <c r="B116" t="s">
-        <v>46</v>
-      </c>
-      <c r="C116">
+      <c r="B116" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C116" s="2">
         <v>5303.97</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="2">
         <v>35647.56</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="2">
         <v>40951.53</v>
       </c>
     </row>
     <row r="117" spans="1:17">
-      <c r="B117" t="s">
-        <v>47</v>
-      </c>
-      <c r="C117">
+      <c r="B117" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C117" s="2">
         <v>16.96</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="2">
         <v>83.04</v>
       </c>
+      <c r="E117" s="2"/>
     </row>
     <row r="118" spans="1:17">
-      <c r="B118" t="s">
-        <v>48</v>
-      </c>
-      <c r="C118">
+      <c r="B118" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C118" s="2">
         <v>57.86</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="2">
         <v>42.14</v>
       </c>
+      <c r="E118" s="2"/>
     </row>
     <row r="121" spans="1:17">
-      <c r="C121" t="s">
-        <v>49</v>
-      </c>
-      <c r="H121" t="s">
-        <v>54</v>
-      </c>
-      <c r="M121" t="s">
-        <v>55</v>
-      </c>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="L121" s="2"/>
+      <c r="M121" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N121" s="2"/>
+      <c r="O121" s="2"/>
     </row>
     <row r="122" spans="1:17">
-      <c r="B122" t="s">
-        <v>50</v>
-      </c>
-      <c r="C122" t="s">
-        <v>51</v>
-      </c>
-      <c r="D122" t="s">
-        <v>52</v>
-      </c>
-      <c r="E122" t="s">
-        <v>53</v>
-      </c>
-      <c r="G122" t="s">
-        <v>50</v>
-      </c>
-      <c r="H122" t="s">
-        <v>51</v>
-      </c>
-      <c r="I122" t="s">
-        <v>52</v>
-      </c>
-      <c r="J122" t="s">
-        <v>53</v>
-      </c>
-      <c r="L122" t="s">
-        <v>50</v>
-      </c>
-      <c r="M122" t="s">
-        <v>51</v>
-      </c>
-      <c r="N122" t="s">
-        <v>52</v>
-      </c>
-      <c r="O122" t="s">
-        <v>53</v>
+      <c r="B122" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H122" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I122" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J122" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M122" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N122" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O122" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="123" spans="1:17">
-      <c r="B123">
+      <c r="B123" s="2">
         <v>693</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="2">
         <v>616</v>
       </c>
-      <c r="D123">
+      <c r="D123" s="2">
         <v>0</v>
       </c>
-      <c r="E123">
+      <c r="E123" s="2">
         <v>0</v>
       </c>
-      <c r="G123">
+      <c r="G123" s="2">
         <v>644</v>
       </c>
-      <c r="H123">
+      <c r="H123" s="2">
         <v>265</v>
       </c>
-      <c r="I123">
+      <c r="I123" s="2">
         <v>0</v>
       </c>
-      <c r="J123">
+      <c r="J123" s="2">
         <v>0</v>
       </c>
-      <c r="L123">
+      <c r="L123" s="2">
         <v>1337</v>
       </c>
-      <c r="M123">
+      <c r="M123" s="2">
         <v>881</v>
       </c>
-      <c r="N123">
+      <c r="N123" s="2">
         <v>0</v>
       </c>
-      <c r="O123">
+      <c r="O123" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:17">
       <c r="H141" s="12" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="142" spans="1:17">
-      <c r="B142" t="s">
-        <v>57</v>
-      </c>
-      <c r="D142" t="s">
-        <v>58</v>
-      </c>
-      <c r="E142" t="s">
-        <v>59</v>
+      <c r="B142" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="143" spans="1:17">
-      <c r="C143" t="s">
+      <c r="B143" s="2"/>
+      <c r="C143" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D143" s="2">
+        <v>7046068.58</v>
+      </c>
+      <c r="E143" s="2">
+        <v>68.87</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17">
+      <c r="B144" s="2"/>
+      <c r="C144" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D144" s="2">
+        <v>1466</v>
+      </c>
+      <c r="E144" s="2">
+        <v>76.0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17">
+      <c r="B145" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="I145" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J145" s="2"/>
+      <c r="K145" s="2"/>
+      <c r="L145" s="2"/>
+      <c r="M145" s="2"/>
+      <c r="N145" s="2"/>
+      <c r="O145" s="2"/>
+    </row>
+    <row r="146" spans="1:17">
+      <c r="B146" s="2"/>
+      <c r="C146" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D146" s="2">
+        <v>7014508</v>
+      </c>
+      <c r="E146" s="2">
+        <v>31561</v>
+      </c>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D143">
-        <v>7046068.58</v>
-      </c>
-      <c r="E143">
-        <v>68.87</v>
-      </c>
-    </row>
-    <row r="144" spans="1:17">
-      <c r="C144" t="s">
-        <v>45</v>
-      </c>
-      <c r="D144">
-        <v>1466</v>
-      </c>
-      <c r="E144">
-        <v>76.0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17">
-      <c r="B145" t="s">
-        <v>60</v>
-      </c>
-      <c r="I145" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17">
-      <c r="C146" t="s">
-        <v>44</v>
-      </c>
-      <c r="D146">
-        <v>7014508</v>
-      </c>
-      <c r="E146">
-        <v>31561</v>
-      </c>
-      <c r="J146" t="s">
-        <v>63</v>
-      </c>
-      <c r="K146">
+      <c r="K146" s="2">
         <v>1459</v>
       </c>
-      <c r="L146">
+      <c r="L146" s="2">
         <v>7</v>
       </c>
+      <c r="M146" s="2"/>
+      <c r="N146" s="2"/>
+      <c r="O146" s="2"/>
     </row>
     <row r="147" spans="1:17">
-      <c r="C147" t="s">
-        <v>61</v>
-      </c>
-      <c r="D147"/>
-      <c r="E147">
+      <c r="B147" s="2"/>
+      <c r="C147" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2">
         <v>35</v>
       </c>
-      <c r="J147" t="s">
-        <v>61</v>
-      </c>
-      <c r="K147"/>
-      <c r="L147">
+      <c r="I147" s="2"/>
+      <c r="J147" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K147" s="2"/>
+      <c r="L147" s="2">
         <v>35</v>
       </c>
+      <c r="M147" s="2"/>
+      <c r="N147" s="2"/>
+      <c r="O147" s="2"/>
     </row>
     <row r="151" spans="1:17">
       <c r="B151" s="2"/>
@@ -5033,180 +5119,136 @@
       <c r="O161" s="2"/>
     </row>
     <row r="167" spans="1:17">
-      <c r="C167" t="s">
+      <c r="B167" s="2"/>
+      <c r="C167" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F167" t="s">
+      <c r="F167" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G167" t="s">
+      <c r="G167" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H167" t="s">
+      <c r="H167" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I167" t="s">
+      <c r="I167" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J167" t="s">
+      <c r="J167" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K167" t="s">
+      <c r="K167" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L167" t="s">
+      <c r="L167" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M167" t="s">
+      <c r="M167" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N167" t="s">
+      <c r="N167" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O167" t="s">
+      <c r="O167" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:17">
-      <c r="B168" t="s">
-        <v>64</v>
-      </c>
-      <c r="C168">
+      <c r="B168" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C168" s="2">
         <v>131</v>
       </c>
-      <c r="D168">
+      <c r="D168" s="2">
         <v>174</v>
       </c>
-      <c r="E168">
+      <c r="E168" s="2">
         <v>223</v>
       </c>
-      <c r="F168">
+      <c r="F168" s="2">
         <v>161</v>
       </c>
-      <c r="G168">
+      <c r="G168" s="2">
         <v>171</v>
       </c>
-      <c r="H168">
+      <c r="H168" s="2">
         <v>249</v>
       </c>
-      <c r="I168">
+      <c r="I168" s="2">
         <v>204</v>
       </c>
-      <c r="J168">
+      <c r="J168" s="2">
         <v>115</v>
       </c>
-      <c r="K168">
+      <c r="K168" s="2">
         <v>167</v>
       </c>
-      <c r="L168">
+      <c r="L168" s="2">
         <v>269</v>
       </c>
-      <c r="M168">
+      <c r="M168" s="2">
         <v>199</v>
       </c>
-      <c r="N168">
+      <c r="N168" s="2">
         <v>251</v>
       </c>
-      <c r="O168">
+      <c r="O168" s="2">
         <f>SUM(C168:N168)</f>
         <v>2314</v>
       </c>
     </row>
     <row r="169" spans="1:17">
-      <c r="B169" t="s">
-        <v>65</v>
-      </c>
-      <c r="C169">
+      <c r="B169" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C169" s="2">
         <v>75.0</v>
       </c>
-      <c r="D169">
+      <c r="D169" s="2">
         <v>73.2919</v>
       </c>
-      <c r="E169">
+      <c r="E169" s="2">
         <v>71.3636</v>
       </c>
-      <c r="F169">
+      <c r="F169" s="2">
         <v>77.6923</v>
       </c>
-      <c r="G169">
+      <c r="G169" s="2">
         <v>82.2222</v>
       </c>
-      <c r="H169">
+      <c r="H169" s="2">
         <v>79.0476</v>
       </c>
-      <c r="I169">
+      <c r="I169" s="2">
         <v>69.7802</v>
       </c>
-      <c r="J169">
+      <c r="J169" s="2">
         <v>72.9412</v>
       </c>
-      <c r="K169">
+      <c r="K169" s="2">
         <v>76.0331</v>
       </c>
-      <c r="L169">
-        <v>77.1552</v>
-      </c>
-      <c r="M169">
+      <c r="L169" s="2">
+        <v>77.4892</v>
+      </c>
+      <c r="M169" s="2">
         <v>70.6587</v>
       </c>
-      <c r="N169">
+      <c r="N169" s="2">
         <v>78.6458</v>
       </c>
-      <c r="O169">
+      <c r="O169" s="2">
         <f>SUM(C169:N169) / 12</f>
-        <v>75.319316666667</v>
-      </c>
-    </row>
-    <row r="180" spans="1:17">
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
-      <c r="D180" s="2"/>
-      <c r="E180" s="2"/>
-    </row>
-    <row r="181" spans="1:17">
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
-      <c r="D181" s="2"/>
-      <c r="E181" s="2"/>
-    </row>
-    <row r="182" spans="1:17">
-      <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
-      <c r="D182" s="2"/>
-      <c r="E182" s="2"/>
-    </row>
-    <row r="183" spans="1:17">
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
-      <c r="D183" s="2"/>
-      <c r="E183" s="2"/>
-      <c r="I183" s="2"/>
-      <c r="J183" s="2"/>
-      <c r="K183" s="2"/>
-    </row>
-    <row r="184" spans="1:17">
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
-      <c r="D184" s="2"/>
-      <c r="E184" s="2"/>
-      <c r="I184" s="2"/>
-      <c r="J184" s="2"/>
-      <c r="K184" s="2"/>
-    </row>
-    <row r="185" spans="1:17">
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
-      <c r="D185" s="2"/>
-      <c r="E185" s="2"/>
-      <c r="I185" s="2"/>
-      <c r="J185" s="2"/>
-      <c r="K185" s="2"/>
+        <v>75.34715</v>
+      </c>
     </row>
     <row r="205" spans="1:17">
       <c r="B205" s="2"/>

</xml_diff>